<commit_message>
logo update and .command file to start app
</commit_message>
<xml_diff>
--- a/sunset-calc-performance.xlsx
+++ b/sunset-calc-performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/938fa7904acb035c/Uni Bern/EC-yield_and_charring_calculation_R/R skript development/sunset-calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{0D0B52DA-14A4-9140-8D77-65AF9CACC0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BBB7DD33-8C29-9349-9584-9F961990146F}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{0D0B52DA-14A4-9140-8D77-65AF9CACC0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E2D439C-F0C8-9640-8E9E-DF7819B4E172}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="1" xr2:uid="{37B338B3-0D50-6C40-A204-80C8EAE19EE4}"/>
   </bookViews>
@@ -19,9 +19,6 @@
     <sheet name="calc 426" sheetId="1" r:id="rId4"/>
     <sheet name="tc-calc" sheetId="7" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="164">
   <si>
     <t>Sample ID</t>
   </si>
@@ -458,6 +455,81 @@
   </si>
   <si>
     <t>online</t>
+  </si>
+  <si>
+    <t>B169_170_OC</t>
+  </si>
+  <si>
+    <t>B171_172_OC</t>
+  </si>
+  <si>
+    <t>UD20_DOC_1</t>
+  </si>
+  <si>
+    <t>UD20_DOC_2</t>
+  </si>
+  <si>
+    <t>UD20_DOC_3</t>
+  </si>
+  <si>
+    <t>C15a</t>
+  </si>
+  <si>
+    <t>C15b</t>
+  </si>
+  <si>
+    <t>C15c</t>
+  </si>
+  <si>
+    <t>C15d</t>
+  </si>
+  <si>
+    <t>C15e</t>
+  </si>
+  <si>
+    <t>C15f</t>
+  </si>
+  <si>
+    <t>c21a</t>
+  </si>
+  <si>
+    <t>c21b</t>
+  </si>
+  <si>
+    <t>c21c</t>
+  </si>
+  <si>
+    <t>c21d</t>
+  </si>
+  <si>
+    <t>c21e</t>
+  </si>
+  <si>
+    <t>c21f</t>
+  </si>
+  <si>
+    <t>I2-A</t>
+  </si>
+  <si>
+    <t>I2-B</t>
+  </si>
+  <si>
+    <t>I3-A</t>
+  </si>
+  <si>
+    <t>I3-B</t>
+  </si>
+  <si>
+    <t>B2-A</t>
+  </si>
+  <si>
+    <t>B2-B</t>
+  </si>
+  <si>
+    <t>B3-A</t>
+  </si>
+  <si>
+    <t>B3-B</t>
   </si>
 </sst>
 </file>
@@ -6919,1950 +6991,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="summary"/>
-      <sheetName val="oc-calc"/>
-      <sheetName val="oc removal calc 426"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>Sunset calc426</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>oc-calc</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>1</v>
-          </cell>
-          <cell r="C5">
-            <v>9.3416169999999994</v>
-          </cell>
-          <cell r="D5">
-            <v>7.8288919999999997</v>
-          </cell>
-          <cell r="F5">
-            <v>7.64516228346627</v>
-          </cell>
-          <cell r="I5">
-            <v>9.4752998103076695</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>2</v>
-          </cell>
-          <cell r="C6">
-            <v>7.2615369999999997</v>
-          </cell>
-          <cell r="D6">
-            <v>6.124352</v>
-          </cell>
-          <cell r="F6">
-            <v>5.9277329058260699</v>
-          </cell>
-          <cell r="I6">
-            <v>7.5774307838808896</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>3</v>
-          </cell>
-          <cell r="C7">
-            <v>7.5905649999999998</v>
-          </cell>
-          <cell r="D7">
-            <v>6.2947800000000003</v>
-          </cell>
-          <cell r="F7">
-            <v>6.0904152906381599</v>
-          </cell>
-          <cell r="I7">
-            <v>7.7996163730385497</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>4</v>
-          </cell>
-          <cell r="C8">
-            <v>6.5020980000000002</v>
-          </cell>
-          <cell r="D8">
-            <v>5.5145879999999998</v>
-          </cell>
-          <cell r="F8">
-            <v>5.3033946016594999</v>
-          </cell>
-          <cell r="I8">
-            <v>6.77510995403573</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>5</v>
-          </cell>
-          <cell r="C9">
-            <v>7.7969949999999999</v>
-          </cell>
-          <cell r="D9">
-            <v>6.5332280000000003</v>
-          </cell>
-          <cell r="F9">
-            <v>6.3586994823353997</v>
-          </cell>
-          <cell r="I9">
-            <v>8.0945489506160904</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>6</v>
-          </cell>
-          <cell r="C10">
-            <v>5.4851340000000004</v>
-          </cell>
-          <cell r="D10">
-            <v>4.6232379999999997</v>
-          </cell>
-          <cell r="F10">
-            <v>4.3910193669257396</v>
-          </cell>
-          <cell r="I10">
-            <v>5.7640569842021003</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>7</v>
-          </cell>
-          <cell r="C11">
-            <v>6.5481829999999999</v>
-          </cell>
-          <cell r="D11">
-            <v>5.3924709999999996</v>
-          </cell>
-          <cell r="F11">
-            <v>5.1770898379231696</v>
-          </cell>
-          <cell r="I11">
-            <v>6.8021783239298799</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>8</v>
-          </cell>
-          <cell r="C12">
-            <v>6.436388</v>
-          </cell>
-          <cell r="D12">
-            <v>5.34537</v>
-          </cell>
-          <cell r="F12">
-            <v>5.1275921612237703</v>
-          </cell>
-          <cell r="I12">
-            <v>6.7102739701639802</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>9</v>
-          </cell>
-          <cell r="C13">
-            <v>5.490507</v>
-          </cell>
-          <cell r="D13">
-            <v>4.5695360000000003</v>
-          </cell>
-          <cell r="F13">
-            <v>4.3510449148305996</v>
-          </cell>
-          <cell r="I13">
-            <v>5.7772645568943899</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>10</v>
-          </cell>
-          <cell r="C14">
-            <v>8.3578709999999994</v>
-          </cell>
-          <cell r="D14">
-            <v>6.9876379999999996</v>
-          </cell>
-          <cell r="F14">
-            <v>6.8026195730192098</v>
-          </cell>
-          <cell r="I14">
-            <v>8.6644645454847904</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>11</v>
-          </cell>
-          <cell r="C15">
-            <v>8.0453569999999992</v>
-          </cell>
-          <cell r="D15">
-            <v>6.8020420000000001</v>
-          </cell>
-          <cell r="F15">
-            <v>6.6147196573884397</v>
-          </cell>
-          <cell r="I15">
-            <v>8.3330976525975693</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>12</v>
-          </cell>
-          <cell r="C16">
-            <v>8.5765840000000004</v>
-          </cell>
-          <cell r="D16">
-            <v>7.0866429999999996</v>
-          </cell>
-          <cell r="F16">
-            <v>6.9148866224269403</v>
-          </cell>
-          <cell r="I16">
-            <v>8.8878526072948691</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>13</v>
-          </cell>
-          <cell r="C17">
-            <v>44.342115</v>
-          </cell>
-          <cell r="D17">
-            <v>21.019665</v>
-          </cell>
-          <cell r="E17">
-            <v>21.495000000000001</v>
-          </cell>
-          <cell r="F17">
-            <v>21.578455823031799</v>
-          </cell>
-          <cell r="I17">
-            <v>45.081150511992497</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>14</v>
-          </cell>
-          <cell r="C18">
-            <v>47.399924999999996</v>
-          </cell>
-          <cell r="D18">
-            <v>22.779555000000002</v>
-          </cell>
-          <cell r="E18">
-            <v>23.25</v>
-          </cell>
-          <cell r="F18">
-            <v>23.368837944750901</v>
-          </cell>
-          <cell r="I18">
-            <v>48.102248109097602</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>15</v>
-          </cell>
-          <cell r="C19">
-            <v>25.088940000000001</v>
-          </cell>
-          <cell r="D19">
-            <v>12.271258500000002</v>
-          </cell>
-          <cell r="E19">
-            <v>12.585000000000001</v>
-          </cell>
-          <cell r="F19">
-            <v>12.3560695988222</v>
-          </cell>
-          <cell r="I19">
-            <v>25.307015851641001</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>16</v>
-          </cell>
-          <cell r="C20">
-            <v>33.604785</v>
-          </cell>
-          <cell r="D20">
-            <v>15.687570000000001</v>
-          </cell>
-          <cell r="E20">
-            <v>16.065000000000001</v>
-          </cell>
-          <cell r="F20">
-            <v>15.9824477630102</v>
-          </cell>
-          <cell r="I20">
-            <v>34.129042883679098</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>17</v>
-          </cell>
-          <cell r="C21">
-            <v>25.307115000000003</v>
-          </cell>
-          <cell r="D21">
-            <v>14.108352</v>
-          </cell>
-          <cell r="E21">
-            <v>14.385</v>
-          </cell>
-          <cell r="F21">
-            <v>14.225807300977801</v>
-          </cell>
-          <cell r="I21">
-            <v>25.638608363467799</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>18</v>
-          </cell>
-          <cell r="C22">
-            <v>41.681775000000002</v>
-          </cell>
-          <cell r="D22">
-            <v>18.979904999999999</v>
-          </cell>
-          <cell r="E22">
-            <v>19.365000000000002</v>
-          </cell>
-          <cell r="F22">
-            <v>19.352936634259098</v>
-          </cell>
-          <cell r="I22">
-            <v>42.176102720448696</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>19</v>
-          </cell>
-          <cell r="C23">
-            <v>60.306659999999994</v>
-          </cell>
-          <cell r="D23">
-            <v>29.464844999999997</v>
-          </cell>
-          <cell r="E23">
-            <v>29.924999999999997</v>
-          </cell>
-          <cell r="F23">
-            <v>30.304088923466701</v>
-          </cell>
-          <cell r="I23">
-            <v>61.454026673819598</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>20</v>
-          </cell>
-          <cell r="C24">
-            <v>69.89605499999999</v>
-          </cell>
-          <cell r="D24">
-            <v>33.416865000000001</v>
-          </cell>
-          <cell r="E24">
-            <v>33.96</v>
-          </cell>
-          <cell r="F24">
-            <v>34.218255270157201</v>
-          </cell>
-          <cell r="I24">
-            <v>70.757994039570903</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>21</v>
-          </cell>
-          <cell r="C25">
-            <v>23.427524999999999</v>
-          </cell>
-          <cell r="D25">
-            <v>12.848647500000002</v>
-          </cell>
-          <cell r="E25">
-            <v>13.169999999999998</v>
-          </cell>
-          <cell r="F25">
-            <v>12.941615988852</v>
-          </cell>
-          <cell r="I25">
-            <v>23.783326488728498</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>22</v>
-          </cell>
-          <cell r="C26">
-            <v>62.947659999999999</v>
-          </cell>
-          <cell r="D26">
-            <v>42.202820000000003</v>
-          </cell>
-          <cell r="E26">
-            <v>43.75</v>
-          </cell>
-          <cell r="F26">
-            <v>43.900629600000002</v>
-          </cell>
-          <cell r="I26">
-            <v>64.477045500000003</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>23</v>
-          </cell>
-          <cell r="C27">
-            <v>72.583299999999994</v>
-          </cell>
-          <cell r="D27">
-            <v>51.88944</v>
-          </cell>
-          <cell r="E27">
-            <v>52.69</v>
-          </cell>
-          <cell r="F27">
-            <v>53.969000299999998</v>
-          </cell>
-          <cell r="I27">
-            <v>74.657956499999997</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>24</v>
-          </cell>
-          <cell r="C28">
-            <v>10.97115</v>
-          </cell>
-          <cell r="D28">
-            <v>6.8992329999999997</v>
-          </cell>
-          <cell r="E28">
-            <v>7.23</v>
-          </cell>
-          <cell r="F28">
-            <v>7.1408380999999999</v>
-          </cell>
-          <cell r="I28">
-            <v>12.114296299999999</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>25</v>
-          </cell>
-          <cell r="C29">
-            <v>10.43554</v>
-          </cell>
-          <cell r="D29">
-            <v>6.0720669999999997</v>
-          </cell>
-          <cell r="E29">
-            <v>6.9</v>
-          </cell>
-          <cell r="F29">
-            <v>6.3994012800000002</v>
-          </cell>
-          <cell r="I29">
-            <v>11.511521200000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>26</v>
-          </cell>
-          <cell r="C30">
-            <v>7.8915889999999997</v>
-          </cell>
-          <cell r="D30">
-            <v>4.6044989999999997</v>
-          </cell>
-          <cell r="E30">
-            <v>5.21</v>
-          </cell>
-          <cell r="F30">
-            <v>4.8257350399999996</v>
-          </cell>
-          <cell r="I30">
-            <v>8.9807561699999994</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>27</v>
-          </cell>
-          <cell r="C31">
-            <v>11.91028</v>
-          </cell>
-          <cell r="D31">
-            <v>7.0946210000000001</v>
-          </cell>
-          <cell r="F31">
-            <v>7.0199729094582501</v>
-          </cell>
-          <cell r="I31">
-            <v>12.257365242631201</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>28</v>
-          </cell>
-          <cell r="C32">
-            <v>10.735810000000001</v>
-          </cell>
-          <cell r="D32">
-            <v>6.2839710000000002</v>
-          </cell>
-          <cell r="F32">
-            <v>6.2159493667140699</v>
-          </cell>
-          <cell r="I32">
-            <v>11.2154141708367</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>29</v>
-          </cell>
-          <cell r="C33">
-            <v>17.871510000000001</v>
-          </cell>
-          <cell r="D33">
-            <v>10.46766</v>
-          </cell>
-          <cell r="F33">
-            <v>10.5574866355562</v>
-          </cell>
-          <cell r="I33">
-            <v>18.3958793683979</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>30</v>
-          </cell>
-          <cell r="C34">
-            <v>12.5076</v>
-          </cell>
-          <cell r="D34">
-            <v>7.1612650000000002</v>
-          </cell>
-          <cell r="F34">
-            <v>7.0404311774692303</v>
-          </cell>
-          <cell r="I34">
-            <v>12.695737837217701</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>31</v>
-          </cell>
-          <cell r="C35">
-            <v>15.500249999999999</v>
-          </cell>
-          <cell r="D35">
-            <v>8.7222380000000008</v>
-          </cell>
-          <cell r="F35">
-            <v>8.6971705841872993</v>
-          </cell>
-          <cell r="I35">
-            <v>15.7876619819379</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>32</v>
-          </cell>
-          <cell r="C36">
-            <v>14.52591</v>
-          </cell>
-          <cell r="D36">
-            <v>8.3235650000000003</v>
-          </cell>
-          <cell r="F36">
-            <v>8.2625402115639393</v>
-          </cell>
-          <cell r="I36">
-            <v>14.8242568204651</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>33</v>
-          </cell>
-          <cell r="C37">
-            <v>19.684190000000001</v>
-          </cell>
-          <cell r="D37">
-            <v>11.09346</v>
-          </cell>
-          <cell r="F37">
-            <v>11.2590684210234</v>
-          </cell>
-          <cell r="I37">
-            <v>20.251701290898499</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>34</v>
-          </cell>
-          <cell r="C38">
-            <v>22.196149999999999</v>
-          </cell>
-          <cell r="D38">
-            <v>11.82222</v>
-          </cell>
-          <cell r="F38">
-            <v>11.8962368180913</v>
-          </cell>
-          <cell r="I38">
-            <v>22.5868446387646</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>35</v>
-          </cell>
-          <cell r="C39">
-            <v>19.999199999999998</v>
-          </cell>
-          <cell r="D39">
-            <v>11.175660000000001</v>
-          </cell>
-          <cell r="F39">
-            <v>11.2551358124015</v>
-          </cell>
-          <cell r="I39">
-            <v>20.421603412645901</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>36</v>
-          </cell>
-          <cell r="C40">
-            <v>14.60826</v>
-          </cell>
-          <cell r="D40">
-            <v>8.4396380000000004</v>
-          </cell>
-          <cell r="F40">
-            <v>8.4307510268964698</v>
-          </cell>
-          <cell r="I40">
-            <v>15.0070954418642</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>37</v>
-          </cell>
-          <cell r="C41">
-            <v>19.23751</v>
-          </cell>
-          <cell r="D41">
-            <v>11.32023</v>
-          </cell>
-          <cell r="F41">
-            <v>11.3795421970253</v>
-          </cell>
-          <cell r="I41">
-            <v>19.627653570056101</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>38</v>
-          </cell>
-          <cell r="C42">
-            <v>15.54016</v>
-          </cell>
-          <cell r="D42">
-            <v>9.4975129999999996</v>
-          </cell>
-          <cell r="F42">
-            <v>9.4774831990038901</v>
-          </cell>
-          <cell r="I42">
-            <v>15.8563228305926</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>39</v>
-          </cell>
-          <cell r="C44">
-            <v>36.494719800000006</v>
-          </cell>
-          <cell r="F44">
-            <v>22.187363586039201</v>
-          </cell>
-          <cell r="I44">
-            <v>36.894241801173997</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>40</v>
-          </cell>
-          <cell r="C45">
-            <v>14.3188507</v>
-          </cell>
-          <cell r="F45">
-            <v>8.5167511631081592</v>
-          </cell>
-          <cell r="I45">
-            <v>14.3835691966099</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>41</v>
-          </cell>
-          <cell r="C46">
-            <v>29.803281200000001</v>
-          </cell>
-          <cell r="F46">
-            <v>17.704507947759598</v>
-          </cell>
-          <cell r="I46">
-            <v>30.0573457695148</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>42</v>
-          </cell>
-          <cell r="C47">
-            <v>27.222272</v>
-          </cell>
-          <cell r="F47">
-            <v>16.637349617478598</v>
-          </cell>
-          <cell r="I47">
-            <v>27.4027366862097</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>43</v>
-          </cell>
-          <cell r="C48">
-            <v>22.303134700000001</v>
-          </cell>
-          <cell r="F48">
-            <v>14.558773156429501</v>
-          </cell>
-          <cell r="I48">
-            <v>22.507826127476299</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>44</v>
-          </cell>
-          <cell r="C49">
-            <v>11.169627699999999</v>
-          </cell>
-          <cell r="F49">
-            <v>6.4695157867401196</v>
-          </cell>
-          <cell r="I49">
-            <v>11.2236820111792</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>45</v>
-          </cell>
-          <cell r="C50">
-            <v>51.508826600000006</v>
-          </cell>
-          <cell r="F50">
-            <v>30.049946834390401</v>
-          </cell>
-          <cell r="I50">
-            <v>52.123402176601502</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>46</v>
-          </cell>
-          <cell r="C51">
-            <v>50.571998399999998</v>
-          </cell>
-          <cell r="F51">
-            <v>30.388644899913398</v>
-          </cell>
-          <cell r="I51">
-            <v>51.266235546455299</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="B3">
-            <v>7.64516228346627</v>
-          </cell>
-          <cell r="C3">
-            <v>0.23344383195310101</v>
-          </cell>
-          <cell r="D3">
-            <v>0.52414376360363901</v>
-          </cell>
-          <cell r="E3">
-            <v>9.4752998103076695</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>5.9277329058260699</v>
-          </cell>
-          <cell r="C4">
-            <v>0.13416313192412499</v>
-          </cell>
-          <cell r="D4">
-            <v>0.44297977618377898</v>
-          </cell>
-          <cell r="E4">
-            <v>7.5774307838808896</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>6.0904152906381599</v>
-          </cell>
-          <cell r="C5">
-            <v>0.17591366234203801</v>
-          </cell>
-          <cell r="D5">
-            <v>0.46073303776514402</v>
-          </cell>
-          <cell r="E5">
-            <v>7.7996163730385497</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>5.3033946016594999</v>
-          </cell>
-          <cell r="C6">
-            <v>6.3644148616411503E-2</v>
-          </cell>
-          <cell r="D6">
-            <v>0.33554418197694702</v>
-          </cell>
-          <cell r="E6">
-            <v>6.77510995403573</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>6.3586994823353997</v>
-          </cell>
-          <cell r="C7">
-            <v>0.23702495507251101</v>
-          </cell>
-          <cell r="D7">
-            <v>0.426271373334699</v>
-          </cell>
-          <cell r="E7">
-            <v>8.0945489506160904</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>4.3910193669257396</v>
-          </cell>
-          <cell r="C8">
-            <v>2.6291174669911498E-2</v>
-          </cell>
-          <cell r="D8">
-            <v>0.27418783088445697</v>
-          </cell>
-          <cell r="E8">
-            <v>5.7640569842021003</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>5.1770898379231696</v>
-          </cell>
-          <cell r="C9">
-            <v>0.149364182367379</v>
-          </cell>
-          <cell r="D9">
-            <v>0.40315398834600402</v>
-          </cell>
-          <cell r="E9">
-            <v>6.8021783239298799</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>5.1275921612237703</v>
-          </cell>
-          <cell r="C10">
-            <v>0.10560889900628399</v>
-          </cell>
-          <cell r="D10">
-            <v>0.40451715839345898</v>
-          </cell>
-          <cell r="E10">
-            <v>6.7102739701639802</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>4.3510449148305996</v>
-          </cell>
-          <cell r="C11">
-            <v>5.1172661009649102E-2</v>
-          </cell>
-          <cell r="D11">
-            <v>0.30249019232374302</v>
-          </cell>
-          <cell r="E11">
-            <v>5.7772645568943899</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>6.8026195730192098</v>
-          </cell>
-          <cell r="C12">
-            <v>0.29029597719523798</v>
-          </cell>
-          <cell r="D12">
-            <v>0.49881351358710702</v>
-          </cell>
-          <cell r="E12">
-            <v>8.6644645454847904</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>6.6147196573884397</v>
-          </cell>
-          <cell r="C13">
-            <v>0.22231334304047801</v>
-          </cell>
-          <cell r="D13">
-            <v>0.423558165580042</v>
-          </cell>
-          <cell r="E13">
-            <v>8.3330976525975693</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>6.9148866224269403</v>
-          </cell>
-          <cell r="C14">
-            <v>0.32369212143055198</v>
-          </cell>
-          <cell r="D14">
-            <v>0.57671568079125302</v>
-          </cell>
-          <cell r="E14">
-            <v>8.8878526072948691</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>21.578455823031799</v>
-          </cell>
-          <cell r="C18">
-            <v>12.0422801198327</v>
-          </cell>
-          <cell r="D18">
-            <v>10.388072802108701</v>
-          </cell>
-          <cell r="E18">
-            <v>45.081150511992497</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>23.368837944750901</v>
-          </cell>
-          <cell r="C19">
-            <v>12.2718616156703</v>
-          </cell>
-          <cell r="D19">
-            <v>11.388997482632201</v>
-          </cell>
-          <cell r="E19">
-            <v>48.102248109097602</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>12.3560695988222</v>
-          </cell>
-          <cell r="C20">
-            <v>6.0364923453842803</v>
-          </cell>
-          <cell r="D20">
-            <v>5.8418309804238602</v>
-          </cell>
-          <cell r="E20">
-            <v>25.307015851641001</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>15.9824477630102</v>
-          </cell>
-          <cell r="C21">
-            <v>8.1738441973006903</v>
-          </cell>
-          <cell r="D21">
-            <v>8.9002350844556197</v>
-          </cell>
-          <cell r="E21">
-            <v>34.129042883679098</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>14.225807300977801</v>
-          </cell>
-          <cell r="C22">
-            <v>5.44731041439971</v>
-          </cell>
-          <cell r="D22">
-            <v>4.8929307555670496</v>
-          </cell>
-          <cell r="E22">
-            <v>25.638608363467799</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>19.352936634259098</v>
-          </cell>
-          <cell r="C23">
-            <v>10.705026757651201</v>
-          </cell>
-          <cell r="D23">
-            <v>11.0454911622409</v>
-          </cell>
-          <cell r="E23">
-            <v>42.176102720448696</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>30.304088923466701</v>
-          </cell>
-          <cell r="C24">
-            <v>15.2322695453612</v>
-          </cell>
-          <cell r="D24">
-            <v>14.8450794493922</v>
-          </cell>
-          <cell r="E24">
-            <v>61.454026673819598</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>34.218255270157201</v>
-          </cell>
-          <cell r="C25">
-            <v>17.108706115012101</v>
-          </cell>
-          <cell r="D25">
-            <v>18.358490421564198</v>
-          </cell>
-          <cell r="E25">
-            <v>70.757994039570903</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>12.941615988852</v>
-          </cell>
-          <cell r="C26">
-            <v>4.8499103344311401</v>
-          </cell>
-          <cell r="D26">
-            <v>4.9192294800115102</v>
-          </cell>
-          <cell r="E26">
-            <v>23.783326488728498</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>43.900629600000002</v>
-          </cell>
-          <cell r="C30">
-            <v>10.013116200000001</v>
-          </cell>
-          <cell r="D30">
-            <v>9.6987925599999993</v>
-          </cell>
-          <cell r="E30">
-            <v>64.477045500000003</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>53.969000299999998</v>
-          </cell>
-          <cell r="C31">
-            <v>10.5746591</v>
-          </cell>
-          <cell r="D31">
-            <v>9.2498413799999994</v>
-          </cell>
-          <cell r="E31">
-            <v>74.657956499999997</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>7.1408380999999999</v>
-          </cell>
-          <cell r="C32">
-            <v>1.69713033</v>
-          </cell>
-          <cell r="D32">
-            <v>2.4118096000000002</v>
-          </cell>
-          <cell r="E32">
-            <v>12.114296299999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>6.3994012800000002</v>
-          </cell>
-          <cell r="C33">
-            <v>1.75715719</v>
-          </cell>
-          <cell r="D33">
-            <v>2.4904498899999998</v>
-          </cell>
-          <cell r="E33">
-            <v>11.511521200000001</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>4.8257350399999996</v>
-          </cell>
-          <cell r="C34">
-            <v>1.2612048899999999</v>
-          </cell>
-          <cell r="D34">
-            <v>2.0292841300000002</v>
-          </cell>
-          <cell r="E34">
-            <v>8.9807561699999994</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>7.0199729094582501</v>
-          </cell>
-          <cell r="C38">
-            <v>2.24455294921195</v>
-          </cell>
-          <cell r="D38">
-            <v>1.92027855414723</v>
-          </cell>
-          <cell r="E38">
-            <v>12.257365242631201</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>6.2159493667140699</v>
-          </cell>
-          <cell r="C39">
-            <v>2.0640324758409001</v>
-          </cell>
-          <cell r="D39">
-            <v>1.8628363890991499</v>
-          </cell>
-          <cell r="E39">
-            <v>11.2154141708367</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>10.5574866355562</v>
-          </cell>
-          <cell r="C40">
-            <v>4.2630729993340504</v>
-          </cell>
-          <cell r="D40">
-            <v>2.5027651278019598</v>
-          </cell>
-          <cell r="E40">
-            <v>18.3958793683979</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>7.0404311774692303</v>
-          </cell>
-          <cell r="C41">
-            <v>2.3135668006228198</v>
-          </cell>
-          <cell r="D41">
-            <v>2.2691746483484199</v>
-          </cell>
-          <cell r="E41">
-            <v>12.695737837217701</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>8.6971705841872993</v>
-          </cell>
-          <cell r="C42">
-            <v>3.5099533370258098</v>
-          </cell>
-          <cell r="D42">
-            <v>2.5079875087666998</v>
-          </cell>
-          <cell r="E42">
-            <v>15.7876619819379</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>8.2625402115639393</v>
-          </cell>
-          <cell r="C43">
-            <v>2.9013817748876298</v>
-          </cell>
-          <cell r="D43">
-            <v>2.5878165616258499</v>
-          </cell>
-          <cell r="E43">
-            <v>14.8242568204651</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>11.2590684210234</v>
-          </cell>
-          <cell r="C44">
-            <v>4.79624887501154</v>
-          </cell>
-          <cell r="D44">
-            <v>3.1238344224115</v>
-          </cell>
-          <cell r="E44">
-            <v>20.251701290898499</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>11.8962368180913</v>
-          </cell>
-          <cell r="C45">
-            <v>5.1084630785340996</v>
-          </cell>
-          <cell r="D45">
-            <v>4.5097769211522198</v>
-          </cell>
-          <cell r="E45">
-            <v>22.5868446387646</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>11.2551358124015</v>
-          </cell>
-          <cell r="C46">
-            <v>4.3381682745413404</v>
-          </cell>
-          <cell r="D46">
-            <v>3.7557320850454801</v>
-          </cell>
-          <cell r="E46">
-            <v>20.421603412645901</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>8.4307510268964698</v>
-          </cell>
-          <cell r="C47">
-            <v>2.8613663514165402</v>
-          </cell>
-          <cell r="D47">
-            <v>2.642411803725</v>
-          </cell>
-          <cell r="E47">
-            <v>15.0070954418642</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>11.3795421970253</v>
-          </cell>
-          <cell r="C48">
-            <v>3.9387137372505201</v>
-          </cell>
-          <cell r="D48">
-            <v>3.23650766278358</v>
-          </cell>
-          <cell r="E48">
-            <v>19.627653570056101</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>9.4774831990038901</v>
-          </cell>
-          <cell r="C49">
-            <v>2.90177888449342</v>
-          </cell>
-          <cell r="D49">
-            <v>2.4045115800327301</v>
-          </cell>
-          <cell r="E49">
-            <v>15.8563228305926</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>22.187363586039201</v>
-          </cell>
-          <cell r="C53">
-            <v>5.0034555307900304</v>
-          </cell>
-          <cell r="D53">
-            <v>8.7903510136621108</v>
-          </cell>
-          <cell r="E53">
-            <v>36.894241801173997</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>8.5167511631081592</v>
-          </cell>
-          <cell r="C54">
-            <v>1.9668871909516601</v>
-          </cell>
-          <cell r="D54">
-            <v>2.9866561298502501</v>
-          </cell>
-          <cell r="E54">
-            <v>14.3835691966099</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>17.704507947759598</v>
-          </cell>
-          <cell r="C55">
-            <v>5.8448626074521899</v>
-          </cell>
-          <cell r="D55">
-            <v>5.5949295377662898</v>
-          </cell>
-          <cell r="E55">
-            <v>30.0573457695148</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>16.637349617478598</v>
-          </cell>
-          <cell r="C56">
-            <v>4.9496144234325996</v>
-          </cell>
-          <cell r="D56">
-            <v>4.9027255049806104</v>
-          </cell>
-          <cell r="E56">
-            <v>27.4027366862097</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>14.558773156429501</v>
-          </cell>
-          <cell r="C57">
-            <v>3.4231449136740699</v>
-          </cell>
-          <cell r="D57">
-            <v>3.6125851863057701</v>
-          </cell>
-          <cell r="E57">
-            <v>22.507826127476299</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58">
-            <v>6.4695157867401196</v>
-          </cell>
-          <cell r="C58">
-            <v>1.5172150494338501</v>
-          </cell>
-          <cell r="D58">
-            <v>2.3238986199068399</v>
-          </cell>
-          <cell r="E58">
-            <v>11.2236820111792</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59">
-            <v>30.049946834390401</v>
-          </cell>
-          <cell r="C59">
-            <v>11.904879256189</v>
-          </cell>
-          <cell r="D59">
-            <v>9.2526595406910506</v>
-          </cell>
-          <cell r="E59">
-            <v>52.123402176601502</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>30.388644899913398</v>
-          </cell>
-          <cell r="C60">
-            <v>11.607438200328</v>
-          </cell>
-          <cell r="D60">
-            <v>8.3571517250305902</v>
-          </cell>
-          <cell r="E60">
-            <v>51.266235546455299</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="5">
-          <cell r="I5">
-            <v>9.3416169999999994</v>
-          </cell>
-          <cell r="V5">
-            <v>7.8288919999999997</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>7.2615369999999997</v>
-          </cell>
-          <cell r="V6">
-            <v>6.124352</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="I7">
-            <v>7.5905649999999998</v>
-          </cell>
-          <cell r="V7">
-            <v>6.2947800000000003</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="I8">
-            <v>6.5020980000000002</v>
-          </cell>
-          <cell r="V8">
-            <v>5.5145879999999998</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="I9">
-            <v>7.7969949999999999</v>
-          </cell>
-          <cell r="V9">
-            <v>6.5332280000000003</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="I10">
-            <v>5.4851340000000004</v>
-          </cell>
-          <cell r="V10">
-            <v>4.6232379999999997</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="I11">
-            <v>6.5481829999999999</v>
-          </cell>
-          <cell r="V11">
-            <v>5.3924709999999996</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="I12">
-            <v>6.436388</v>
-          </cell>
-          <cell r="V12">
-            <v>5.34537</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="I13">
-            <v>5.490507</v>
-          </cell>
-          <cell r="V13">
-            <v>4.5695360000000003</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="I14">
-            <v>8.3578709999999994</v>
-          </cell>
-          <cell r="V14">
-            <v>6.9876379999999996</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="I15">
-            <v>8.0453569999999992</v>
-          </cell>
-          <cell r="V15">
-            <v>6.8020420000000001</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="I16">
-            <v>8.5765840000000004</v>
-          </cell>
-          <cell r="V16">
-            <v>7.0866429999999996</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="I23">
-            <v>29.561409999999999</v>
-          </cell>
-          <cell r="V23">
-            <v>14.013109999999999</v>
-          </cell>
-          <cell r="AD23">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="I24">
-            <v>31.59995</v>
-          </cell>
-          <cell r="V24">
-            <v>15.18637</v>
-          </cell>
-          <cell r="AD24">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="I25">
-            <v>16.725960000000001</v>
-          </cell>
-          <cell r="V25">
-            <v>8.1808390000000006</v>
-          </cell>
-          <cell r="AD25">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="I26">
-            <v>22.403189999999999</v>
-          </cell>
-          <cell r="V26">
-            <v>10.45838</v>
-          </cell>
-          <cell r="AD26">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="I27">
-            <v>16.871410000000001</v>
-          </cell>
-          <cell r="V27">
-            <v>9.4055680000000006</v>
-          </cell>
-          <cell r="AD27">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="I28">
-            <v>27.787849999999999</v>
-          </cell>
-          <cell r="V28">
-            <v>12.653269999999999</v>
-          </cell>
-          <cell r="AD28">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="I29">
-            <v>40.204439999999998</v>
-          </cell>
-          <cell r="V29">
-            <v>19.643229999999999</v>
-          </cell>
-          <cell r="AD29">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="I30">
-            <v>46.597369999999998</v>
-          </cell>
-          <cell r="V30">
-            <v>22.277909999999999</v>
-          </cell>
-          <cell r="AD30">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="I31">
-            <v>15.61835</v>
-          </cell>
-          <cell r="V31">
-            <v>8.5657650000000007</v>
-          </cell>
-          <cell r="AD31">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>UD20_DOC_1</v>
-          </cell>
-          <cell r="I45">
-            <v>10.97115</v>
-          </cell>
-          <cell r="V45">
-            <v>6.8992329999999997</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>UD20_DOC_2</v>
-          </cell>
-          <cell r="I46">
-            <v>10.43554</v>
-          </cell>
-          <cell r="V46">
-            <v>6.0720669999999997</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>UD20_DOC_3</v>
-          </cell>
-          <cell r="I47">
-            <v>7.8915889999999997</v>
-          </cell>
-          <cell r="V47">
-            <v>4.6044989999999997</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>B169_170_OC</v>
-          </cell>
-          <cell r="I57">
-            <v>62.947659999999999</v>
-          </cell>
-          <cell r="V57">
-            <v>42.202820000000003</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>B171_172_OC</v>
-          </cell>
-          <cell r="I59">
-            <v>72.583299999999994</v>
-          </cell>
-          <cell r="V59">
-            <v>51.88944</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>C15a</v>
-          </cell>
-          <cell r="I78">
-            <v>11.91028</v>
-          </cell>
-          <cell r="V78">
-            <v>7.0946210000000001</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>C15b</v>
-          </cell>
-          <cell r="I79">
-            <v>10.735810000000001</v>
-          </cell>
-          <cell r="V79">
-            <v>6.2839710000000002</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80" t="str">
-            <v>C15c</v>
-          </cell>
-          <cell r="I80">
-            <v>17.871510000000001</v>
-          </cell>
-          <cell r="V80">
-            <v>10.46766</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81" t="str">
-            <v>C15d</v>
-          </cell>
-          <cell r="I81">
-            <v>12.5076</v>
-          </cell>
-          <cell r="V81">
-            <v>7.1612650000000002</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82" t="str">
-            <v>C15e</v>
-          </cell>
-          <cell r="I82">
-            <v>15.500249999999999</v>
-          </cell>
-          <cell r="V82">
-            <v>8.7222380000000008</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83" t="str">
-            <v>C15f</v>
-          </cell>
-          <cell r="I83">
-            <v>14.52591</v>
-          </cell>
-          <cell r="V83">
-            <v>8.3235650000000003</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84" t="str">
-            <v>c21a</v>
-          </cell>
-          <cell r="I84">
-            <v>19.684190000000001</v>
-          </cell>
-          <cell r="V84">
-            <v>11.09346</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85" t="str">
-            <v>c21b</v>
-          </cell>
-          <cell r="I85">
-            <v>22.196149999999999</v>
-          </cell>
-          <cell r="V85">
-            <v>11.82222</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86" t="str">
-            <v>c21c</v>
-          </cell>
-          <cell r="I86">
-            <v>19.999199999999998</v>
-          </cell>
-          <cell r="V86">
-            <v>11.175660000000001</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87" t="str">
-            <v>c21d</v>
-          </cell>
-          <cell r="I87">
-            <v>14.60826</v>
-          </cell>
-          <cell r="V87">
-            <v>8.4396380000000004</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88" t="str">
-            <v>c21e</v>
-          </cell>
-          <cell r="I88">
-            <v>19.23751</v>
-          </cell>
-          <cell r="V88">
-            <v>11.32023</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89" t="str">
-            <v>c21f</v>
-          </cell>
-          <cell r="I89">
-            <v>15.54016</v>
-          </cell>
-          <cell r="V89">
-            <v>9.4975129999999996</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96" t="str">
-            <v>I2-A</v>
-          </cell>
-          <cell r="I96">
-            <v>47.395740000000004</v>
-          </cell>
-          <cell r="Z96">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97" t="str">
-            <v>I2-B</v>
-          </cell>
-          <cell r="I97">
-            <v>18.59591</v>
-          </cell>
-          <cell r="Z97">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98" t="str">
-            <v>I3-A</v>
-          </cell>
-          <cell r="I98">
-            <v>38.705559999999998</v>
-          </cell>
-          <cell r="Z98">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99" t="str">
-            <v>I3-B</v>
-          </cell>
-          <cell r="I99">
-            <v>35.3536</v>
-          </cell>
-          <cell r="Z99">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100" t="str">
-            <v>B2-A</v>
-          </cell>
-          <cell r="I100">
-            <v>28.965109999999999</v>
-          </cell>
-          <cell r="Z100">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101" t="str">
-            <v>B2-B</v>
-          </cell>
-          <cell r="I101">
-            <v>14.50601</v>
-          </cell>
-          <cell r="Z101">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102" t="str">
-            <v>B3-A</v>
-          </cell>
-          <cell r="I102">
-            <v>66.894580000000005</v>
-          </cell>
-          <cell r="Z102">
-            <v>0.77</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103" t="str">
-            <v>B3-B</v>
-          </cell>
-          <cell r="I103">
-            <v>65.67792</v>
-          </cell>
-          <cell r="Z103">
-            <v>0.77</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ThemeMR-standard_Arial">
   <a:themeElements>
@@ -10218,7 +8346,7 @@
         <v>10.356051705707801</v>
       </c>
       <c r="E5" s="20">
-        <f>(100*D5/C5)-100</f>
+        <f t="shared" ref="E5:E28" si="0">(100*D5/C5)-100</f>
         <v>-2.4886024876035151</v>
       </c>
       <c r="F5" s="5"/>
@@ -10243,7 +8371,7 @@
         <v>5.1188933571202497</v>
       </c>
       <c r="E6" s="20">
-        <f>(100*D6/C6)-100</f>
+        <f t="shared" si="0"/>
         <v>-5.7400625947590953</v>
       </c>
       <c r="F6" s="5"/>
@@ -10268,7 +8396,7 @@
         <v>3.0896033405308398</v>
       </c>
       <c r="E7" s="20">
-        <f>(100*D7/C7)-100</f>
+        <f t="shared" si="0"/>
         <v>-10.336344546187348</v>
       </c>
       <c r="F7" s="5"/>
@@ -10293,7 +8421,7 @@
         <v>11.9949869878815</v>
       </c>
       <c r="E8" s="20">
-        <f>(100*D8/C8)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.795293784003789</v>
       </c>
       <c r="F8" s="5"/>
@@ -10318,7 +8446,7 @@
         <v>82.100635395858205</v>
       </c>
       <c r="E9" s="20">
-        <f>(100*D9/C9)-100</f>
+        <f t="shared" si="0"/>
         <v>1.6205384731121057</v>
       </c>
       <c r="F9" s="5"/>
@@ -10343,7 +8471,7 @@
         <v>8.6552110485417693</v>
       </c>
       <c r="E10" s="20">
-        <f>(100*D10/C10)-100</f>
+        <f t="shared" si="0"/>
         <v>-2.881100769125112</v>
       </c>
       <c r="F10" s="5"/>
@@ -10368,7 +8496,7 @@
         <v>11.711977586352701</v>
       </c>
       <c r="E11" s="20">
-        <f>(100*D11/C11)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.517798565819092</v>
       </c>
       <c r="F11" s="5"/>
@@ -10393,7 +8521,7 @@
         <v>60.9794299136082</v>
       </c>
       <c r="E12" s="20">
-        <f>(100*D12/C12)-100</f>
+        <f t="shared" si="0"/>
         <v>1.418162675236232</v>
       </c>
       <c r="F12" s="5"/>
@@ -10418,7 +8546,7 @@
         <v>40.034381783222898</v>
       </c>
       <c r="E13" s="20">
-        <f>(100*D13/C13)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2966007823069816</v>
       </c>
       <c r="F13" s="5"/>
@@ -10443,7 +8571,7 @@
         <v>12.167757773437501</v>
       </c>
       <c r="E14" s="20">
-        <f>(100*D14/C14)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.5828644539638788</v>
       </c>
       <c r="F14" s="5"/>
@@ -10468,7 +8596,7 @@
         <v>11.8067738377901</v>
       </c>
       <c r="E15" s="20">
-        <f>(100*D15/C15)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.4916385783545536</v>
       </c>
       <c r="F15" s="5"/>
@@ -10493,7 +8621,7 @@
         <v>22.936186828068401</v>
       </c>
       <c r="E16" s="20">
-        <f>(100*D16/C16)-100</f>
+        <f t="shared" si="0"/>
         <v>0.24763108362979835</v>
       </c>
       <c r="F16" s="5"/>
@@ -10518,7 +8646,7 @@
         <v>101.40145478911801</v>
       </c>
       <c r="E17" s="20">
-        <f>(100*D17/C17)-100</f>
+        <f t="shared" si="0"/>
         <v>1.5176823836790732</v>
       </c>
       <c r="F17" s="5"/>
@@ -10543,7 +8671,7 @@
         <v>71.139656497189307</v>
       </c>
       <c r="E18" s="20">
-        <f>(100*D18/C18)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3760887183134827</v>
       </c>
       <c r="F18" s="5"/>
@@ -10568,7 +8696,7 @@
         <v>49.413172398329003</v>
       </c>
       <c r="E19" s="20">
-        <f>(100*D19/C19)-100</f>
+        <f t="shared" si="0"/>
         <v>1.1736959511600702</v>
       </c>
       <c r="F19" s="5"/>
@@ -10593,7 +8721,7 @@
         <v>38.757677613311301</v>
       </c>
       <c r="E20" s="20">
-        <f>(100*D20/C20)-100</f>
+        <f t="shared" si="0"/>
         <v>1.0320895509493226</v>
       </c>
       <c r="F20" s="5"/>
@@ -10617,7 +8745,7 @@
         <v>46.371621918929797</v>
       </c>
       <c r="E21" s="20">
-        <f>(100*D21/C21)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2335719103359821</v>
       </c>
       <c r="F21" s="5"/>
@@ -10639,7 +8767,7 @@
         <v>85.947777828096307</v>
       </c>
       <c r="E22" s="20">
-        <f>(100*D22/C22)-100</f>
+        <f t="shared" si="0"/>
         <v>1.678625397322989</v>
       </c>
       <c r="F22" s="5"/>
@@ -10661,7 +8789,7 @@
         <v>32.043392802293198</v>
       </c>
       <c r="E23" s="20">
-        <f>(100*D23/C23)-100</f>
+        <f t="shared" si="0"/>
         <v>0.75317222485512048</v>
       </c>
       <c r="F23" s="5"/>
@@ -10683,7 +8811,7 @@
         <v>63.690081365730101</v>
       </c>
       <c r="E24" s="20">
-        <f>(100*D24/C24)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3600860051407295</v>
       </c>
       <c r="F24" s="5"/>
@@ -10705,7 +8833,7 @@
         <v>39.648048558367698</v>
       </c>
       <c r="E25" s="20">
-        <f>(100*D25/C25)-100</f>
+        <f t="shared" si="0"/>
         <v>1.0529356325287296</v>
       </c>
       <c r="F25" s="5"/>
@@ -10727,7 +8855,7 @@
         <v>93.9731484911443</v>
       </c>
       <c r="E26" s="20">
-        <f>(100*D26/C26)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3538416625445393</v>
       </c>
       <c r="F26" s="5"/>
@@ -10750,7 +8878,7 @@
         <v>45.629335815583801</v>
       </c>
       <c r="E27" s="20">
-        <f>(100*D27/C27)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2173449871037434</v>
       </c>
       <c r="G27" s="5"/>
@@ -10772,7 +8900,7 @@
         <v>77.199122637166695</v>
       </c>
       <c r="E28" s="20">
-        <f>(100*D28/C28)-100</f>
+        <f t="shared" si="0"/>
         <v>1.4571790472335806</v>
       </c>
       <c r="G28" s="5"/>
@@ -10805,7 +8933,7 @@
         <v>91.004236169929797</v>
       </c>
       <c r="E30" s="20">
-        <f>(100*D30/C30)-100</f>
+        <f t="shared" ref="E30:E35" si="1">(100*D30/C30)-100</f>
         <v>1.9808535601033128</v>
       </c>
       <c r="G30" s="5"/>
@@ -10828,7 +8956,7 @@
         <v>131.10605604278501</v>
       </c>
       <c r="E31" s="20">
-        <f>(100*D31/C31)-100</f>
+        <f t="shared" si="1"/>
         <v>1.7339333129448278</v>
       </c>
       <c r="G31" s="5"/>
@@ -10851,7 +8979,7 @@
         <v>114.85910233806899</v>
       </c>
       <c r="E32" s="20">
-        <f>(100*D32/C32)-100</f>
+        <f t="shared" si="1"/>
         <v>1.8207740363586851</v>
       </c>
       <c r="G32" s="5"/>
@@ -10874,7 +9002,7 @@
         <v>177.81723146532099</v>
       </c>
       <c r="E33" s="20">
-        <f>(100*D33/C33)-100</f>
+        <f t="shared" si="1"/>
         <v>1.9188061324879016</v>
       </c>
       <c r="F33" s="5"/>
@@ -10898,7 +9026,7 @@
         <v>66.456130976349399</v>
       </c>
       <c r="E34" s="20">
-        <f>(100*D34/C34)-100</f>
+        <f t="shared" si="1"/>
         <v>1.7920346639202904</v>
       </c>
       <c r="F34" s="5"/>
@@ -10922,7 +9050,7 @@
         <v>74.977355399024205</v>
       </c>
       <c r="E35" s="20">
-        <f>(100*D35/C35)-100</f>
+        <f t="shared" si="1"/>
         <v>1.8325692891640415</v>
       </c>
       <c r="F35" s="5"/>
@@ -11179,7 +9307,7 @@
         <v>3.0896033405308398</v>
       </c>
       <c r="E5" s="20">
-        <f>(100*D5/C5)-100</f>
+        <f t="shared" ref="E5:E34" si="0">(100*D5/C5)-100</f>
         <v>-10.336344546187348</v>
       </c>
       <c r="F5" s="5"/>
@@ -11204,7 +9332,7 @@
         <v>5.1188933571202497</v>
       </c>
       <c r="E6" s="20">
-        <f>(100*D6/C6)-100</f>
+        <f t="shared" si="0"/>
         <v>-5.7400625947590953</v>
       </c>
       <c r="F6" s="5"/>
@@ -11229,7 +9357,7 @@
         <v>8.6552110485417693</v>
       </c>
       <c r="E7" s="20">
-        <f>(100*D7/C7)-100</f>
+        <f t="shared" si="0"/>
         <v>-2.881100769125112</v>
       </c>
       <c r="F7" s="5"/>
@@ -11254,7 +9382,7 @@
         <v>10.356051705707801</v>
       </c>
       <c r="E8" s="20">
-        <f>(100*D8/C8)-100</f>
+        <f t="shared" si="0"/>
         <v>-2.4886024876035151</v>
       </c>
       <c r="F8" s="5"/>
@@ -11279,7 +9407,7 @@
         <v>11.711977586352701</v>
       </c>
       <c r="E9" s="20">
-        <f>(100*D9/C9)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.517798565819092</v>
       </c>
       <c r="F9" s="5"/>
@@ -11304,7 +9432,7 @@
         <v>11.8067738377901</v>
       </c>
       <c r="E10" s="20">
-        <f>(100*D10/C10)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.4916385783545536</v>
       </c>
       <c r="F10" s="5"/>
@@ -11329,7 +9457,7 @@
         <v>11.9949869878815</v>
       </c>
       <c r="E11" s="20">
-        <f>(100*D11/C11)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.795293784003789</v>
       </c>
       <c r="F11" s="5"/>
@@ -11354,7 +9482,7 @@
         <v>12.167757773437501</v>
       </c>
       <c r="E12" s="20">
-        <f>(100*D12/C12)-100</f>
+        <f t="shared" si="0"/>
         <v>-1.5828644539638788</v>
       </c>
       <c r="F12" s="5"/>
@@ -11379,7 +9507,7 @@
         <v>22.936186828068401</v>
       </c>
       <c r="E13" s="20">
-        <f>(100*D13/C13)-100</f>
+        <f t="shared" si="0"/>
         <v>0.24763108362979835</v>
       </c>
       <c r="F13" s="5"/>
@@ -11403,7 +9531,7 @@
         <v>32.043392802293198</v>
       </c>
       <c r="E14" s="20">
-        <f>(100*D14/C14)-100</f>
+        <f t="shared" si="0"/>
         <v>0.75317222485512048</v>
       </c>
       <c r="F14" s="5"/>
@@ -11428,7 +9556,7 @@
         <v>38.757677613311301</v>
       </c>
       <c r="E15" s="20">
-        <f>(100*D15/C15)-100</f>
+        <f t="shared" si="0"/>
         <v>1.0320895509493226</v>
       </c>
       <c r="F15" s="5"/>
@@ -11452,7 +9580,7 @@
         <v>39.648048558367698</v>
       </c>
       <c r="E16" s="20">
-        <f>(100*D16/C16)-100</f>
+        <f t="shared" si="0"/>
         <v>1.0529356325287296</v>
       </c>
       <c r="F16" s="5"/>
@@ -11477,7 +9605,7 @@
         <v>40.034381783222898</v>
       </c>
       <c r="E17" s="20">
-        <f>(100*D17/C17)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2966007823069816</v>
       </c>
       <c r="F17" s="5"/>
@@ -11501,7 +9629,7 @@
         <v>45.629335815583801</v>
       </c>
       <c r="E18" s="20">
-        <f>(100*D18/C18)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2173449871037434</v>
       </c>
       <c r="F18" s="5"/>
@@ -11525,7 +9653,7 @@
         <v>46.371621918929797</v>
       </c>
       <c r="E19" s="20">
-        <f>(100*D19/C19)-100</f>
+        <f t="shared" si="0"/>
         <v>1.2335719103359821</v>
       </c>
       <c r="F19" s="5"/>
@@ -11550,7 +9678,7 @@
         <v>49.413172398329003</v>
       </c>
       <c r="E20" s="20">
-        <f>(100*D20/C20)-100</f>
+        <f t="shared" si="0"/>
         <v>1.1736959511600702</v>
       </c>
       <c r="F20" s="5"/>
@@ -11575,7 +9703,7 @@
         <v>60.9794299136082</v>
       </c>
       <c r="E21" s="20">
-        <f>(100*D21/C21)-100</f>
+        <f t="shared" si="0"/>
         <v>1.418162675236232</v>
       </c>
       <c r="F21" s="5"/>
@@ -11597,7 +9725,7 @@
         <v>63.690081365730101</v>
       </c>
       <c r="E22" s="20">
-        <f>(100*D22/C22)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3600860051407295</v>
       </c>
       <c r="F22" s="5"/>
@@ -11620,7 +9748,7 @@
         <v>66.456130976349399</v>
       </c>
       <c r="E23" s="20">
-        <f>(100*D23/C23)-100</f>
+        <f t="shared" si="0"/>
         <v>1.7920346639202904</v>
       </c>
       <c r="F23" s="5"/>
@@ -11643,7 +9771,7 @@
         <v>71.139656497189307</v>
       </c>
       <c r="E24" s="20">
-        <f>(100*D24/C24)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3760887183134827</v>
       </c>
       <c r="F24" s="5"/>
@@ -11666,7 +9794,7 @@
         <v>74.977355399024205</v>
       </c>
       <c r="E25" s="20">
-        <f>(100*D25/C25)-100</f>
+        <f t="shared" si="0"/>
         <v>1.8325692891640415</v>
       </c>
       <c r="F25" s="5"/>
@@ -11688,7 +9816,7 @@
         <v>77.199122637166695</v>
       </c>
       <c r="E26" s="20">
-        <f>(100*D26/C26)-100</f>
+        <f t="shared" si="0"/>
         <v>1.4571790472335806</v>
       </c>
       <c r="F26" s="5"/>
@@ -11712,7 +9840,7 @@
         <v>82.100635395858205</v>
       </c>
       <c r="E27" s="20">
-        <f>(100*D27/C27)-100</f>
+        <f t="shared" si="0"/>
         <v>1.6205384731121057</v>
       </c>
       <c r="G27" s="5"/>
@@ -11734,7 +9862,7 @@
         <v>85.947777828096307</v>
       </c>
       <c r="E28" s="20">
-        <f>(100*D28/C28)-100</f>
+        <f t="shared" si="0"/>
         <v>1.678625397322989</v>
       </c>
       <c r="G28" s="5"/>
@@ -11757,7 +9885,7 @@
         <v>91.004236169929797</v>
       </c>
       <c r="E29" s="20">
-        <f>(100*D29/C29)-100</f>
+        <f t="shared" si="0"/>
         <v>1.9808535601033128</v>
       </c>
       <c r="G29" s="5"/>
@@ -11779,7 +9907,7 @@
         <v>93.9731484911443</v>
       </c>
       <c r="E30" s="20">
-        <f>(100*D30/C30)-100</f>
+        <f t="shared" si="0"/>
         <v>1.3538416625445393</v>
       </c>
       <c r="G30" s="5"/>
@@ -11802,7 +9930,7 @@
         <v>101.40145478911801</v>
       </c>
       <c r="E31" s="20">
-        <f>(100*D31/C31)-100</f>
+        <f t="shared" si="0"/>
         <v>1.5176823836790732</v>
       </c>
       <c r="G31" s="5"/>
@@ -11825,7 +9953,7 @@
         <v>114.85910233806899</v>
       </c>
       <c r="E32" s="20">
-        <f>(100*D32/C32)-100</f>
+        <f t="shared" si="0"/>
         <v>1.8207740363586851</v>
       </c>
       <c r="G32" s="5"/>
@@ -11848,7 +9976,7 @@
         <v>131.10605604278501</v>
       </c>
       <c r="E33" s="20">
-        <f>(100*D33/C33)-100</f>
+        <f t="shared" si="0"/>
         <v>1.7339333129448278</v>
       </c>
       <c r="F33" s="5"/>
@@ -11872,7 +10000,7 @@
         <v>177.81723146532099</v>
       </c>
       <c r="E34" s="20">
-        <f>(100*D34/C34)-100</f>
+        <f t="shared" si="0"/>
         <v>1.9188061324879016</v>
       </c>
       <c r="F34" s="5"/>
@@ -12143,28 +10271,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="23">
-        <f>'[1]oc removal calc 426'!I5</f>
         <v>9.3416169999999994</v>
       </c>
       <c r="D5" s="23">
-        <f>'[1]oc removal calc 426'!V5</f>
         <v>7.8288919999999997</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23">
-        <f>'[1]oc-calc'!B3</f>
         <v>7.64516228346627</v>
       </c>
       <c r="G5" s="23">
-        <f>'[1]oc-calc'!C3</f>
         <v>0.23344383195310101</v>
       </c>
       <c r="H5" s="23">
-        <f>'[1]oc-calc'!D3</f>
         <v>0.52414376360363901</v>
       </c>
       <c r="I5" s="23">
-        <f>'[1]oc-calc'!E3</f>
         <v>9.4752998103076695</v>
       </c>
       <c r="J5" s="23"/>
@@ -12177,28 +10299,22 @@
         <v>2</v>
       </c>
       <c r="C6" s="23">
-        <f>'[1]oc removal calc 426'!I6</f>
         <v>7.2615369999999997</v>
       </c>
       <c r="D6" s="23">
-        <f>'[1]oc removal calc 426'!V6</f>
         <v>6.124352</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="23">
-        <f>'[1]oc-calc'!B4</f>
         <v>5.9277329058260699</v>
       </c>
       <c r="G6" s="23">
-        <f>'[1]oc-calc'!C4</f>
         <v>0.13416313192412499</v>
       </c>
       <c r="H6" s="23">
-        <f>'[1]oc-calc'!D4</f>
         <v>0.44297977618377898</v>
       </c>
       <c r="I6" s="23">
-        <f>'[1]oc-calc'!E4</f>
         <v>7.5774307838808896</v>
       </c>
       <c r="J6" s="23"/>
@@ -12211,28 +10327,22 @@
         <v>3</v>
       </c>
       <c r="C7" s="23">
-        <f>'[1]oc removal calc 426'!I7</f>
         <v>7.5905649999999998</v>
       </c>
       <c r="D7" s="23">
-        <f>'[1]oc removal calc 426'!V7</f>
         <v>6.2947800000000003</v>
       </c>
       <c r="E7" s="23"/>
       <c r="F7" s="23">
-        <f>'[1]oc-calc'!B5</f>
         <v>6.0904152906381599</v>
       </c>
       <c r="G7" s="23">
-        <f>'[1]oc-calc'!C5</f>
         <v>0.17591366234203801</v>
       </c>
       <c r="H7" s="23">
-        <f>'[1]oc-calc'!D5</f>
         <v>0.46073303776514402</v>
       </c>
       <c r="I7" s="23">
-        <f>'[1]oc-calc'!E5</f>
         <v>7.7996163730385497</v>
       </c>
       <c r="J7" s="23"/>
@@ -12245,28 +10355,22 @@
         <v>4</v>
       </c>
       <c r="C8" s="23">
-        <f>'[1]oc removal calc 426'!I8</f>
         <v>6.5020980000000002</v>
       </c>
       <c r="D8" s="23">
-        <f>'[1]oc removal calc 426'!V8</f>
         <v>5.5145879999999998</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="23">
-        <f>'[1]oc-calc'!B6</f>
         <v>5.3033946016594999</v>
       </c>
       <c r="G8" s="23">
-        <f>'[1]oc-calc'!C6</f>
         <v>6.3644148616411503E-2</v>
       </c>
       <c r="H8" s="23">
-        <f>'[1]oc-calc'!D6</f>
         <v>0.33554418197694702</v>
       </c>
       <c r="I8" s="23">
-        <f>'[1]oc-calc'!E6</f>
         <v>6.77510995403573</v>
       </c>
       <c r="J8" s="23"/>
@@ -12279,28 +10383,22 @@
         <v>5</v>
       </c>
       <c r="C9" s="23">
-        <f>'[1]oc removal calc 426'!I9</f>
         <v>7.7969949999999999</v>
       </c>
       <c r="D9" s="23">
-        <f>'[1]oc removal calc 426'!V9</f>
         <v>6.5332280000000003</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23">
-        <f>'[1]oc-calc'!B7</f>
         <v>6.3586994823353997</v>
       </c>
       <c r="G9" s="23">
-        <f>'[1]oc-calc'!C7</f>
         <v>0.23702495507251101</v>
       </c>
       <c r="H9" s="23">
-        <f>'[1]oc-calc'!D7</f>
         <v>0.426271373334699</v>
       </c>
       <c r="I9" s="23">
-        <f>'[1]oc-calc'!E7</f>
         <v>8.0945489506160904</v>
       </c>
       <c r="J9" s="23"/>
@@ -12313,28 +10411,22 @@
         <v>6</v>
       </c>
       <c r="C10" s="23">
-        <f>'[1]oc removal calc 426'!I10</f>
         <v>5.4851340000000004</v>
       </c>
       <c r="D10" s="23">
-        <f>'[1]oc removal calc 426'!V10</f>
         <v>4.6232379999999997</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23">
-        <f>'[1]oc-calc'!B8</f>
         <v>4.3910193669257396</v>
       </c>
       <c r="G10" s="23">
-        <f>'[1]oc-calc'!C8</f>
         <v>2.6291174669911498E-2</v>
       </c>
       <c r="H10" s="23">
-        <f>'[1]oc-calc'!D8</f>
         <v>0.27418783088445697</v>
       </c>
       <c r="I10" s="23">
-        <f>'[1]oc-calc'!E8</f>
         <v>5.7640569842021003</v>
       </c>
       <c r="J10" s="23"/>
@@ -12347,28 +10439,22 @@
         <v>7</v>
       </c>
       <c r="C11" s="23">
-        <f>'[1]oc removal calc 426'!I11</f>
         <v>6.5481829999999999</v>
       </c>
       <c r="D11" s="23">
-        <f>'[1]oc removal calc 426'!V11</f>
         <v>5.3924709999999996</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="23">
-        <f>'[1]oc-calc'!B9</f>
         <v>5.1770898379231696</v>
       </c>
       <c r="G11" s="23">
-        <f>'[1]oc-calc'!C9</f>
         <v>0.149364182367379</v>
       </c>
       <c r="H11" s="23">
-        <f>'[1]oc-calc'!D9</f>
         <v>0.40315398834600402</v>
       </c>
       <c r="I11" s="23">
-        <f>'[1]oc-calc'!E9</f>
         <v>6.8021783239298799</v>
       </c>
       <c r="J11" s="23"/>
@@ -12381,28 +10467,22 @@
         <v>8</v>
       </c>
       <c r="C12" s="23">
-        <f>'[1]oc removal calc 426'!I12</f>
         <v>6.436388</v>
       </c>
       <c r="D12" s="23">
-        <f>'[1]oc removal calc 426'!V12</f>
         <v>5.34537</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="23">
-        <f>'[1]oc-calc'!B10</f>
         <v>5.1275921612237703</v>
       </c>
       <c r="G12" s="23">
-        <f>'[1]oc-calc'!C10</f>
         <v>0.10560889900628399</v>
       </c>
       <c r="H12" s="23">
-        <f>'[1]oc-calc'!D10</f>
         <v>0.40451715839345898</v>
       </c>
       <c r="I12" s="23">
-        <f>'[1]oc-calc'!E10</f>
         <v>6.7102739701639802</v>
       </c>
       <c r="J12" s="23"/>
@@ -12415,28 +10495,22 @@
         <v>9</v>
       </c>
       <c r="C13" s="23">
-        <f>'[1]oc removal calc 426'!I13</f>
         <v>5.490507</v>
       </c>
       <c r="D13" s="23">
-        <f>'[1]oc removal calc 426'!V13</f>
         <v>4.5695360000000003</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23">
-        <f>'[1]oc-calc'!B11</f>
         <v>4.3510449148305996</v>
       </c>
       <c r="G13" s="23">
-        <f>'[1]oc-calc'!C11</f>
         <v>5.1172661009649102E-2</v>
       </c>
       <c r="H13" s="23">
-        <f>'[1]oc-calc'!D11</f>
         <v>0.30249019232374302</v>
       </c>
       <c r="I13" s="23">
-        <f>'[1]oc-calc'!E11</f>
         <v>5.7772645568943899</v>
       </c>
       <c r="J13" s="23"/>
@@ -12449,28 +10523,22 @@
         <v>10</v>
       </c>
       <c r="C14" s="23">
-        <f>'[1]oc removal calc 426'!I14</f>
         <v>8.3578709999999994</v>
       </c>
       <c r="D14" s="23">
-        <f>'[1]oc removal calc 426'!V14</f>
         <v>6.9876379999999996</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23">
-        <f>'[1]oc-calc'!B12</f>
         <v>6.8026195730192098</v>
       </c>
       <c r="G14" s="23">
-        <f>'[1]oc-calc'!C12</f>
         <v>0.29029597719523798</v>
       </c>
       <c r="H14" s="23">
-        <f>'[1]oc-calc'!D12</f>
         <v>0.49881351358710702</v>
       </c>
       <c r="I14" s="23">
-        <f>'[1]oc-calc'!E12</f>
         <v>8.6644645454847904</v>
       </c>
       <c r="J14" s="23"/>
@@ -12483,28 +10551,22 @@
         <v>11</v>
       </c>
       <c r="C15" s="23">
-        <f>'[1]oc removal calc 426'!I15</f>
         <v>8.0453569999999992</v>
       </c>
       <c r="D15" s="23">
-        <f>'[1]oc removal calc 426'!V15</f>
         <v>6.8020420000000001</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23">
-        <f>'[1]oc-calc'!B13</f>
         <v>6.6147196573884397</v>
       </c>
       <c r="G15" s="23">
-        <f>'[1]oc-calc'!C13</f>
         <v>0.22231334304047801</v>
       </c>
       <c r="H15" s="23">
-        <f>'[1]oc-calc'!D13</f>
         <v>0.423558165580042</v>
       </c>
       <c r="I15" s="23">
-        <f>'[1]oc-calc'!E13</f>
         <v>8.3330976525975693</v>
       </c>
       <c r="J15" s="23"/>
@@ -12517,28 +10579,22 @@
         <v>12</v>
       </c>
       <c r="C16" s="23">
-        <f>'[1]oc removal calc 426'!I16</f>
         <v>8.5765840000000004</v>
       </c>
       <c r="D16" s="23">
-        <f>'[1]oc removal calc 426'!V16</f>
         <v>7.0866429999999996</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="23">
-        <f>'[1]oc-calc'!B14</f>
         <v>6.9148866224269403</v>
       </c>
       <c r="G16" s="23">
-        <f>'[1]oc-calc'!C14</f>
         <v>0.32369212143055198</v>
       </c>
       <c r="H16" s="23">
-        <f>'[1]oc-calc'!D14</f>
         <v>0.57671568079125302</v>
       </c>
       <c r="I16" s="23">
-        <f>'[1]oc-calc'!E14</f>
         <v>8.8878526072948691</v>
       </c>
       <c r="J16" s="23"/>
@@ -12551,11 +10607,9 @@
         <v>13</v>
       </c>
       <c r="C17" s="23">
-        <f>'[1]oc removal calc 426'!I23*'[1]oc removal calc 426'!AD23</f>
         <v>44.342115</v>
       </c>
       <c r="D17" s="23">
-        <f>'[1]oc removal calc 426'!V23*'[1]oc removal calc 426'!AD23</f>
         <v>21.019665</v>
       </c>
       <c r="E17" s="23">
@@ -12563,19 +10617,15 @@
         <v>21.495000000000001</v>
       </c>
       <c r="F17" s="23">
-        <f>'[1]oc-calc'!B18</f>
         <v>21.578455823031799</v>
       </c>
       <c r="G17" s="23">
-        <f>'[1]oc-calc'!C18</f>
         <v>12.0422801198327</v>
       </c>
       <c r="H17" s="23">
-        <f>'[1]oc-calc'!D18</f>
         <v>10.388072802108701</v>
       </c>
       <c r="I17" s="23">
-        <f>'[1]oc-calc'!E18</f>
         <v>45.081150511992497</v>
       </c>
       <c r="J17" s="23"/>
@@ -12588,11 +10638,9 @@
         <v>14</v>
       </c>
       <c r="C18" s="23">
-        <f>'[1]oc removal calc 426'!I24*'[1]oc removal calc 426'!AD24</f>
         <v>47.399924999999996</v>
       </c>
       <c r="D18" s="23">
-        <f>'[1]oc removal calc 426'!V24*'[1]oc removal calc 426'!AD24</f>
         <v>22.779555000000002</v>
       </c>
       <c r="E18" s="23">
@@ -12600,19 +10648,15 @@
         <v>23.25</v>
       </c>
       <c r="F18" s="23">
-        <f>'[1]oc-calc'!B19</f>
         <v>23.368837944750901</v>
       </c>
       <c r="G18" s="23">
-        <f>'[1]oc-calc'!C19</f>
         <v>12.2718616156703</v>
       </c>
       <c r="H18" s="23">
-        <f>'[1]oc-calc'!D19</f>
         <v>11.388997482632201</v>
       </c>
       <c r="I18" s="23">
-        <f>'[1]oc-calc'!E19</f>
         <v>48.102248109097602</v>
       </c>
       <c r="J18" s="23"/>
@@ -12625,11 +10669,9 @@
         <v>15</v>
       </c>
       <c r="C19" s="23">
-        <f>'[1]oc removal calc 426'!I25*'[1]oc removal calc 426'!AD25</f>
         <v>25.088940000000001</v>
       </c>
       <c r="D19" s="23">
-        <f>'[1]oc removal calc 426'!V25*'[1]oc removal calc 426'!AD25</f>
         <v>12.271258500000002</v>
       </c>
       <c r="E19" s="23">
@@ -12637,19 +10679,15 @@
         <v>12.585000000000001</v>
       </c>
       <c r="F19" s="23">
-        <f>'[1]oc-calc'!B20</f>
         <v>12.3560695988222</v>
       </c>
       <c r="G19" s="23">
-        <f>'[1]oc-calc'!C20</f>
         <v>6.0364923453842803</v>
       </c>
       <c r="H19" s="23">
-        <f>'[1]oc-calc'!D20</f>
         <v>5.8418309804238602</v>
       </c>
       <c r="I19" s="23">
-        <f>'[1]oc-calc'!E20</f>
         <v>25.307015851641001</v>
       </c>
       <c r="J19" s="23"/>
@@ -12662,11 +10700,9 @@
         <v>16</v>
       </c>
       <c r="C20" s="23">
-        <f>'[1]oc removal calc 426'!I26*'[1]oc removal calc 426'!AD26</f>
         <v>33.604785</v>
       </c>
       <c r="D20" s="23">
-        <f>'[1]oc removal calc 426'!V26*'[1]oc removal calc 426'!AD26</f>
         <v>15.687570000000001</v>
       </c>
       <c r="E20" s="23">
@@ -12674,19 +10710,15 @@
         <v>16.065000000000001</v>
       </c>
       <c r="F20" s="23">
-        <f>'[1]oc-calc'!B21</f>
         <v>15.9824477630102</v>
       </c>
       <c r="G20" s="23">
-        <f>'[1]oc-calc'!C21</f>
         <v>8.1738441973006903</v>
       </c>
       <c r="H20" s="23">
-        <f>'[1]oc-calc'!D21</f>
         <v>8.9002350844556197</v>
       </c>
       <c r="I20" s="23">
-        <f>'[1]oc-calc'!E21</f>
         <v>34.129042883679098</v>
       </c>
       <c r="J20" s="23"/>
@@ -12699,11 +10731,9 @@
         <v>17</v>
       </c>
       <c r="C21" s="23">
-        <f>'[1]oc removal calc 426'!I27*'[1]oc removal calc 426'!AD27</f>
         <v>25.307115000000003</v>
       </c>
       <c r="D21" s="23">
-        <f>'[1]oc removal calc 426'!V27*'[1]oc removal calc 426'!AD27</f>
         <v>14.108352</v>
       </c>
       <c r="E21" s="23">
@@ -12711,19 +10741,15 @@
         <v>14.385</v>
       </c>
       <c r="F21" s="23">
-        <f>'[1]oc-calc'!B22</f>
         <v>14.225807300977801</v>
       </c>
       <c r="G21" s="23">
-        <f>'[1]oc-calc'!C22</f>
         <v>5.44731041439971</v>
       </c>
       <c r="H21" s="23">
-        <f>'[1]oc-calc'!D22</f>
         <v>4.8929307555670496</v>
       </c>
       <c r="I21" s="23">
-        <f>'[1]oc-calc'!E22</f>
         <v>25.638608363467799</v>
       </c>
       <c r="J21" s="23"/>
@@ -12736,11 +10762,9 @@
         <v>18</v>
       </c>
       <c r="C22" s="23">
-        <f>'[1]oc removal calc 426'!I28*'[1]oc removal calc 426'!AD28</f>
         <v>41.681775000000002</v>
       </c>
       <c r="D22" s="23">
-        <f>'[1]oc removal calc 426'!V28*'[1]oc removal calc 426'!AD28</f>
         <v>18.979904999999999</v>
       </c>
       <c r="E22" s="23">
@@ -12748,19 +10772,15 @@
         <v>19.365000000000002</v>
       </c>
       <c r="F22" s="23">
-        <f>'[1]oc-calc'!B23</f>
         <v>19.352936634259098</v>
       </c>
       <c r="G22" s="23">
-        <f>'[1]oc-calc'!C23</f>
         <v>10.705026757651201</v>
       </c>
       <c r="H22" s="23">
-        <f>'[1]oc-calc'!D23</f>
         <v>11.0454911622409</v>
       </c>
       <c r="I22" s="23">
-        <f>'[1]oc-calc'!E23</f>
         <v>42.176102720448696</v>
       </c>
       <c r="J22" s="23"/>
@@ -12773,11 +10793,9 @@
         <v>19</v>
       </c>
       <c r="C23" s="23">
-        <f>'[1]oc removal calc 426'!I29*'[1]oc removal calc 426'!AD29</f>
         <v>60.306659999999994</v>
       </c>
       <c r="D23" s="23">
-        <f>'[1]oc removal calc 426'!V29*'[1]oc removal calc 426'!AD29</f>
         <v>29.464844999999997</v>
       </c>
       <c r="E23" s="23">
@@ -12785,19 +10803,15 @@
         <v>29.924999999999997</v>
       </c>
       <c r="F23" s="23">
-        <f>'[1]oc-calc'!B24</f>
         <v>30.304088923466701</v>
       </c>
       <c r="G23" s="23">
-        <f>'[1]oc-calc'!C24</f>
         <v>15.2322695453612</v>
       </c>
       <c r="H23" s="23">
-        <f>'[1]oc-calc'!D24</f>
         <v>14.8450794493922</v>
       </c>
       <c r="I23" s="23">
-        <f>'[1]oc-calc'!E24</f>
         <v>61.454026673819598</v>
       </c>
       <c r="J23" s="23"/>
@@ -12810,11 +10824,9 @@
         <v>20</v>
       </c>
       <c r="C24" s="23">
-        <f>'[1]oc removal calc 426'!I30*'[1]oc removal calc 426'!AD30</f>
         <v>69.89605499999999</v>
       </c>
       <c r="D24" s="23">
-        <f>'[1]oc removal calc 426'!V30*'[1]oc removal calc 426'!AD30</f>
         <v>33.416865000000001</v>
       </c>
       <c r="E24" s="23">
@@ -12822,19 +10834,15 @@
         <v>33.96</v>
       </c>
       <c r="F24" s="23">
-        <f>'[1]oc-calc'!B25</f>
         <v>34.218255270157201</v>
       </c>
       <c r="G24" s="23">
-        <f>'[1]oc-calc'!C25</f>
         <v>17.108706115012101</v>
       </c>
       <c r="H24" s="23">
-        <f>'[1]oc-calc'!D25</f>
         <v>18.358490421564198</v>
       </c>
       <c r="I24" s="23">
-        <f>'[1]oc-calc'!E25</f>
         <v>70.757994039570903</v>
       </c>
       <c r="J24" s="23"/>
@@ -12847,11 +10855,9 @@
         <v>21</v>
       </c>
       <c r="C25" s="23">
-        <f>'[1]oc removal calc 426'!I31*'[1]oc removal calc 426'!AD31</f>
         <v>23.427524999999999</v>
       </c>
       <c r="D25" s="23">
-        <f>'[1]oc removal calc 426'!V31*'[1]oc removal calc 426'!AD31</f>
         <v>12.848647500000002</v>
       </c>
       <c r="E25" s="23">
@@ -12859,601 +10865,478 @@
         <v>13.169999999999998</v>
       </c>
       <c r="F25" s="23">
-        <f>'[1]oc-calc'!B26</f>
         <v>12.941615988852</v>
       </c>
       <c r="G25" s="23">
-        <f>'[1]oc-calc'!C26</f>
         <v>4.8499103344311401</v>
       </c>
       <c r="H25" s="23">
-        <f>'[1]oc-calc'!D26</f>
         <v>4.9192294800115102</v>
       </c>
       <c r="I25" s="23">
-        <f>'[1]oc-calc'!E26</f>
         <v>23.783326488728498</v>
       </c>
       <c r="J25" s="23"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" t="str">
-        <f>'[1]oc removal calc 426'!A57</f>
-        <v>B169_170_OC</v>
+      <c r="A26" t="s">
+        <v>139</v>
       </c>
       <c r="B26">
         <v>22</v>
       </c>
       <c r="C26" s="23">
-        <f>'[1]oc removal calc 426'!$I$57</f>
         <v>62.947659999999999</v>
       </c>
       <c r="D26" s="23">
-        <f>'[1]oc removal calc 426'!$V$57</f>
         <v>42.202820000000003</v>
       </c>
       <c r="E26" s="23">
         <v>43.75</v>
       </c>
       <c r="F26" s="23">
-        <f>'[1]oc-calc'!B30</f>
         <v>43.900629600000002</v>
       </c>
       <c r="G26" s="23">
-        <f>'[1]oc-calc'!C30</f>
         <v>10.013116200000001</v>
       </c>
       <c r="H26" s="23">
-        <f>'[1]oc-calc'!D30</f>
         <v>9.6987925599999993</v>
       </c>
       <c r="I26" s="23">
-        <f>'[1]oc-calc'!E30</f>
         <v>64.477045500000003</v>
       </c>
       <c r="J26" s="23"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" t="str">
-        <f>'[1]oc removal calc 426'!A59</f>
-        <v>B171_172_OC</v>
+      <c r="A27" t="s">
+        <v>140</v>
       </c>
       <c r="B27">
         <v>23</v>
       </c>
       <c r="C27" s="23">
-        <f>'[1]oc removal calc 426'!$I$59</f>
         <v>72.583299999999994</v>
       </c>
       <c r="D27" s="23">
-        <f>'[1]oc removal calc 426'!$V$59</f>
         <v>51.88944</v>
       </c>
       <c r="E27" s="23">
         <v>52.69</v>
       </c>
       <c r="F27" s="23">
-        <f>'[1]oc-calc'!B31</f>
         <v>53.969000299999998</v>
       </c>
       <c r="G27" s="23">
-        <f>'[1]oc-calc'!C31</f>
         <v>10.5746591</v>
       </c>
       <c r="H27" s="23">
-        <f>'[1]oc-calc'!D31</f>
         <v>9.2498413799999994</v>
       </c>
       <c r="I27" s="23">
-        <f>'[1]oc-calc'!E31</f>
         <v>74.657956499999997</v>
       </c>
       <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" t="str">
-        <f>'[1]oc removal calc 426'!A45</f>
-        <v>UD20_DOC_1</v>
+      <c r="A28" t="s">
+        <v>141</v>
       </c>
       <c r="B28">
         <v>24</v>
       </c>
       <c r="C28" s="23">
-        <f>'[1]oc removal calc 426'!$I$45</f>
         <v>10.97115</v>
       </c>
       <c r="D28" s="23">
-        <f>'[1]oc removal calc 426'!$V$45</f>
         <v>6.8992329999999997</v>
       </c>
       <c r="E28" s="23">
         <v>7.23</v>
       </c>
       <c r="F28" s="23">
-        <f>'[1]oc-calc'!B32</f>
         <v>7.1408380999999999</v>
       </c>
       <c r="G28" s="23">
-        <f>'[1]oc-calc'!C32</f>
         <v>1.69713033</v>
       </c>
       <c r="H28" s="23">
-        <f>'[1]oc-calc'!D32</f>
         <v>2.4118096000000002</v>
       </c>
       <c r="I28" s="23">
-        <f>'[1]oc-calc'!E32</f>
         <v>12.114296299999999</v>
       </c>
       <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" t="str">
-        <f>'[1]oc removal calc 426'!A46</f>
-        <v>UD20_DOC_2</v>
+      <c r="A29" t="s">
+        <v>142</v>
       </c>
       <c r="B29">
         <v>25</v>
       </c>
       <c r="C29" s="23">
-        <f>'[1]oc removal calc 426'!$I$46</f>
         <v>10.43554</v>
       </c>
       <c r="D29" s="23">
-        <f>'[1]oc removal calc 426'!$V$46</f>
         <v>6.0720669999999997</v>
       </c>
       <c r="E29" s="23">
         <v>6.9</v>
       </c>
       <c r="F29" s="23">
-        <f>'[1]oc-calc'!B33</f>
         <v>6.3994012800000002</v>
       </c>
       <c r="G29" s="23">
-        <f>'[1]oc-calc'!C33</f>
         <v>1.75715719</v>
       </c>
       <c r="H29" s="23">
-        <f>'[1]oc-calc'!D33</f>
         <v>2.4904498899999998</v>
       </c>
       <c r="I29" s="23">
-        <f>'[1]oc-calc'!E33</f>
         <v>11.511521200000001</v>
       </c>
       <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" t="str">
-        <f>'[1]oc removal calc 426'!A47</f>
-        <v>UD20_DOC_3</v>
+      <c r="A30" t="s">
+        <v>143</v>
       </c>
       <c r="B30">
         <v>26</v>
       </c>
       <c r="C30" s="23">
-        <f>'[1]oc removal calc 426'!$I$47</f>
         <v>7.8915889999999997</v>
       </c>
       <c r="D30" s="23">
-        <f>'[1]oc removal calc 426'!$V$47</f>
         <v>4.6044989999999997</v>
       </c>
       <c r="E30" s="23">
         <v>5.21</v>
       </c>
       <c r="F30" s="23">
-        <f>'[1]oc-calc'!B34</f>
         <v>4.8257350399999996</v>
       </c>
       <c r="G30" s="23">
-        <f>'[1]oc-calc'!C34</f>
         <v>1.2612048899999999</v>
       </c>
       <c r="H30" s="23">
-        <f>'[1]oc-calc'!D34</f>
         <v>2.0292841300000002</v>
       </c>
       <c r="I30" s="23">
-        <f>'[1]oc-calc'!E34</f>
         <v>8.9807561699999994</v>
       </c>
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" t="str">
-        <f>'[1]oc removal calc 426'!A78</f>
-        <v>C15a</v>
+      <c r="A31" t="s">
+        <v>144</v>
       </c>
       <c r="B31">
         <v>27</v>
       </c>
       <c r="C31" s="23">
-        <f>'[1]oc removal calc 426'!I78</f>
         <v>11.91028</v>
       </c>
       <c r="D31" s="23">
-        <f>'[1]oc removal calc 426'!V78</f>
         <v>7.0946210000000001</v>
       </c>
       <c r="F31" s="23">
-        <f>'[1]oc-calc'!B38</f>
         <v>7.0199729094582501</v>
       </c>
       <c r="G31" s="23">
-        <f>'[1]oc-calc'!C38</f>
         <v>2.24455294921195</v>
       </c>
       <c r="H31" s="23">
-        <f>'[1]oc-calc'!D38</f>
         <v>1.92027855414723</v>
       </c>
       <c r="I31" s="23">
-        <f>'[1]oc-calc'!E38</f>
         <v>12.257365242631201</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" t="str">
-        <f>'[1]oc removal calc 426'!A79</f>
-        <v>C15b</v>
+      <c r="A32" t="s">
+        <v>145</v>
       </c>
       <c r="B32">
         <v>28</v>
       </c>
       <c r="C32" s="23">
-        <f>'[1]oc removal calc 426'!I79</f>
         <v>10.735810000000001</v>
       </c>
       <c r="D32" s="23">
-        <f>'[1]oc removal calc 426'!V79</f>
         <v>6.2839710000000002</v>
       </c>
       <c r="F32" s="23">
-        <f>'[1]oc-calc'!B39</f>
         <v>6.2159493667140699</v>
       </c>
       <c r="G32" s="23">
-        <f>'[1]oc-calc'!C39</f>
         <v>2.0640324758409001</v>
       </c>
       <c r="H32" s="23">
-        <f>'[1]oc-calc'!D39</f>
         <v>1.8628363890991499</v>
       </c>
       <c r="I32" s="23">
-        <f>'[1]oc-calc'!E39</f>
         <v>11.2154141708367</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" t="str">
-        <f>'[1]oc removal calc 426'!A80</f>
-        <v>C15c</v>
+      <c r="A33" t="s">
+        <v>146</v>
       </c>
       <c r="B33">
         <v>29</v>
       </c>
       <c r="C33" s="23">
-        <f>'[1]oc removal calc 426'!I80</f>
         <v>17.871510000000001</v>
       </c>
       <c r="D33" s="23">
-        <f>'[1]oc removal calc 426'!V80</f>
         <v>10.46766</v>
       </c>
       <c r="F33" s="23">
-        <f>'[1]oc-calc'!B40</f>
         <v>10.5574866355562</v>
       </c>
       <c r="G33" s="23">
-        <f>'[1]oc-calc'!C40</f>
         <v>4.2630729993340504</v>
       </c>
       <c r="H33" s="23">
-        <f>'[1]oc-calc'!D40</f>
         <v>2.5027651278019598</v>
       </c>
       <c r="I33" s="23">
-        <f>'[1]oc-calc'!E40</f>
         <v>18.3958793683979</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" t="str">
-        <f>'[1]oc removal calc 426'!A81</f>
-        <v>C15d</v>
+      <c r="A34" t="s">
+        <v>147</v>
       </c>
       <c r="B34">
         <v>30</v>
       </c>
       <c r="C34" s="23">
-        <f>'[1]oc removal calc 426'!I81</f>
         <v>12.5076</v>
       </c>
       <c r="D34" s="23">
-        <f>'[1]oc removal calc 426'!V81</f>
         <v>7.1612650000000002</v>
       </c>
       <c r="F34" s="23">
-        <f>'[1]oc-calc'!B41</f>
         <v>7.0404311774692303</v>
       </c>
       <c r="G34" s="23">
-        <f>'[1]oc-calc'!C41</f>
         <v>2.3135668006228198</v>
       </c>
       <c r="H34" s="23">
-        <f>'[1]oc-calc'!D41</f>
         <v>2.2691746483484199</v>
       </c>
       <c r="I34" s="23">
-        <f>'[1]oc-calc'!E41</f>
         <v>12.695737837217701</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" t="str">
-        <f>'[1]oc removal calc 426'!A82</f>
-        <v>C15e</v>
+      <c r="A35" t="s">
+        <v>148</v>
       </c>
       <c r="B35">
         <v>31</v>
       </c>
       <c r="C35" s="23">
-        <f>'[1]oc removal calc 426'!I82</f>
         <v>15.500249999999999</v>
       </c>
       <c r="D35" s="23">
-        <f>'[1]oc removal calc 426'!V82</f>
         <v>8.7222380000000008</v>
       </c>
       <c r="F35" s="23">
-        <f>'[1]oc-calc'!B42</f>
         <v>8.6971705841872993</v>
       </c>
       <c r="G35" s="23">
-        <f>'[1]oc-calc'!C42</f>
         <v>3.5099533370258098</v>
       </c>
       <c r="H35" s="23">
-        <f>'[1]oc-calc'!D42</f>
         <v>2.5079875087666998</v>
       </c>
       <c r="I35" s="23">
-        <f>'[1]oc-calc'!E42</f>
         <v>15.7876619819379</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" t="str">
-        <f>'[1]oc removal calc 426'!A83</f>
-        <v>C15f</v>
+      <c r="A36" t="s">
+        <v>149</v>
       </c>
       <c r="B36">
         <v>32</v>
       </c>
       <c r="C36" s="23">
-        <f>'[1]oc removal calc 426'!I83</f>
         <v>14.52591</v>
       </c>
       <c r="D36" s="23">
-        <f>'[1]oc removal calc 426'!V83</f>
         <v>8.3235650000000003</v>
       </c>
       <c r="F36" s="23">
-        <f>'[1]oc-calc'!B43</f>
         <v>8.2625402115639393</v>
       </c>
       <c r="G36" s="23">
-        <f>'[1]oc-calc'!C43</f>
         <v>2.9013817748876298</v>
       </c>
       <c r="H36" s="23">
-        <f>'[1]oc-calc'!D43</f>
         <v>2.5878165616258499</v>
       </c>
       <c r="I36" s="23">
-        <f>'[1]oc-calc'!E43</f>
         <v>14.8242568204651</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" t="str">
-        <f>'[1]oc removal calc 426'!A84</f>
-        <v>c21a</v>
+      <c r="A37" t="s">
+        <v>150</v>
       </c>
       <c r="B37">
         <v>33</v>
       </c>
       <c r="C37" s="23">
-        <f>'[1]oc removal calc 426'!I84</f>
         <v>19.684190000000001</v>
       </c>
       <c r="D37" s="23">
-        <f>'[1]oc removal calc 426'!V84</f>
         <v>11.09346</v>
       </c>
       <c r="F37" s="23">
-        <f>'[1]oc-calc'!B44</f>
         <v>11.2590684210234</v>
       </c>
       <c r="G37" s="23">
-        <f>'[1]oc-calc'!C44</f>
         <v>4.79624887501154</v>
       </c>
       <c r="H37" s="23">
-        <f>'[1]oc-calc'!D44</f>
         <v>3.1238344224115</v>
       </c>
       <c r="I37" s="23">
-        <f>'[1]oc-calc'!E44</f>
         <v>20.251701290898499</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" t="str">
-        <f>'[1]oc removal calc 426'!A85</f>
-        <v>c21b</v>
+      <c r="A38" t="s">
+        <v>151</v>
       </c>
       <c r="B38">
         <v>34</v>
       </c>
       <c r="C38" s="23">
-        <f>'[1]oc removal calc 426'!I85</f>
         <v>22.196149999999999</v>
       </c>
       <c r="D38" s="23">
-        <f>'[1]oc removal calc 426'!V85</f>
         <v>11.82222</v>
       </c>
       <c r="F38" s="23">
-        <f>'[1]oc-calc'!B45</f>
         <v>11.8962368180913</v>
       </c>
       <c r="G38" s="23">
-        <f>'[1]oc-calc'!C45</f>
         <v>5.1084630785340996</v>
       </c>
       <c r="H38" s="23">
-        <f>'[1]oc-calc'!D45</f>
         <v>4.5097769211522198</v>
       </c>
       <c r="I38" s="23">
-        <f>'[1]oc-calc'!E45</f>
         <v>22.5868446387646</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" t="str">
-        <f>'[1]oc removal calc 426'!A86</f>
-        <v>c21c</v>
+      <c r="A39" t="s">
+        <v>152</v>
       </c>
       <c r="B39">
         <v>35</v>
       </c>
       <c r="C39" s="23">
-        <f>'[1]oc removal calc 426'!I86</f>
         <v>19.999199999999998</v>
       </c>
       <c r="D39" s="23">
-        <f>'[1]oc removal calc 426'!V86</f>
         <v>11.175660000000001</v>
       </c>
       <c r="F39" s="23">
-        <f>'[1]oc-calc'!B46</f>
         <v>11.2551358124015</v>
       </c>
       <c r="G39" s="23">
-        <f>'[1]oc-calc'!C46</f>
         <v>4.3381682745413404</v>
       </c>
       <c r="H39" s="23">
-        <f>'[1]oc-calc'!D46</f>
         <v>3.7557320850454801</v>
       </c>
       <c r="I39" s="23">
-        <f>'[1]oc-calc'!E46</f>
         <v>20.421603412645901</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" t="str">
-        <f>'[1]oc removal calc 426'!A87</f>
-        <v>c21d</v>
+      <c r="A40" t="s">
+        <v>153</v>
       </c>
       <c r="B40">
         <v>36</v>
       </c>
       <c r="C40" s="23">
-        <f>'[1]oc removal calc 426'!I87</f>
         <v>14.60826</v>
       </c>
       <c r="D40" s="23">
-        <f>'[1]oc removal calc 426'!V87</f>
         <v>8.4396380000000004</v>
       </c>
       <c r="F40" s="23">
-        <f>'[1]oc-calc'!B47</f>
         <v>8.4307510268964698</v>
       </c>
       <c r="G40" s="23">
-        <f>'[1]oc-calc'!C47</f>
         <v>2.8613663514165402</v>
       </c>
       <c r="H40" s="23">
-        <f>'[1]oc-calc'!D47</f>
         <v>2.642411803725</v>
       </c>
       <c r="I40" s="23">
-        <f>'[1]oc-calc'!E47</f>
         <v>15.0070954418642</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" t="str">
-        <f>'[1]oc removal calc 426'!A88</f>
-        <v>c21e</v>
+      <c r="A41" t="s">
+        <v>154</v>
       </c>
       <c r="B41">
         <v>37</v>
       </c>
       <c r="C41" s="23">
-        <f>'[1]oc removal calc 426'!I88</f>
         <v>19.23751</v>
       </c>
       <c r="D41" s="23">
-        <f>'[1]oc removal calc 426'!V88</f>
         <v>11.32023</v>
       </c>
       <c r="F41" s="23">
-        <f>'[1]oc-calc'!B48</f>
         <v>11.3795421970253</v>
       </c>
       <c r="G41" s="23">
-        <f>'[1]oc-calc'!C48</f>
         <v>3.9387137372505201</v>
       </c>
       <c r="H41" s="23">
-        <f>'[1]oc-calc'!D48</f>
         <v>3.23650766278358</v>
       </c>
       <c r="I41" s="23">
-        <f>'[1]oc-calc'!E48</f>
         <v>19.627653570056101</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" t="str">
-        <f>'[1]oc removal calc 426'!A89</f>
-        <v>c21f</v>
+      <c r="A42" t="s">
+        <v>155</v>
       </c>
       <c r="B42">
         <v>38</v>
       </c>
       <c r="C42" s="23">
-        <f>'[1]oc removal calc 426'!I89</f>
         <v>15.54016</v>
       </c>
       <c r="D42" s="23">
-        <f>'[1]oc removal calc 426'!V89</f>
         <v>9.4975129999999996</v>
       </c>
       <c r="F42" s="23">
-        <f>'[1]oc-calc'!B49</f>
         <v>9.4774831990038901</v>
       </c>
       <c r="G42" s="23">
-        <f>'[1]oc-calc'!C49</f>
         <v>2.90177888449342</v>
       </c>
       <c r="H42" s="23">
-        <f>'[1]oc-calc'!D49</f>
         <v>2.4045115800327301</v>
       </c>
       <c r="I42" s="23">
-        <f>'[1]oc-calc'!E49</f>
         <v>15.8563228305926</v>
       </c>
     </row>
@@ -13463,242 +11346,194 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" t="str">
-        <f>'[1]oc removal calc 426'!A96</f>
-        <v>I2-A</v>
+      <c r="A44" t="s">
+        <v>156</v>
       </c>
       <c r="B44">
         <v>39</v>
       </c>
       <c r="C44" s="23">
-        <f>'[1]oc removal calc 426'!I96*'[1]oc removal calc 426'!Z96</f>
         <v>36.494719800000006</v>
       </c>
       <c r="D44" s="23"/>
       <c r="F44" s="23">
-        <f>'[1]oc-calc'!B53</f>
         <v>22.187363586039201</v>
       </c>
       <c r="G44" s="23">
-        <f>'[1]oc-calc'!C53</f>
         <v>5.0034555307900304</v>
       </c>
       <c r="H44" s="23">
-        <f>'[1]oc-calc'!D53</f>
         <v>8.7903510136621108</v>
       </c>
       <c r="I44" s="23">
-        <f>'[1]oc-calc'!E53</f>
         <v>36.894241801173997</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" t="str">
-        <f>'[1]oc removal calc 426'!A97</f>
-        <v>I2-B</v>
+      <c r="A45" t="s">
+        <v>157</v>
       </c>
       <c r="B45">
         <v>40</v>
       </c>
       <c r="C45" s="23">
-        <f>'[1]oc removal calc 426'!I97*'[1]oc removal calc 426'!Z97</f>
         <v>14.3188507</v>
       </c>
       <c r="D45" s="23"/>
       <c r="F45" s="23">
-        <f>'[1]oc-calc'!B54</f>
         <v>8.5167511631081592</v>
       </c>
       <c r="G45" s="23">
-        <f>'[1]oc-calc'!C54</f>
         <v>1.9668871909516601</v>
       </c>
       <c r="H45" s="23">
-        <f>'[1]oc-calc'!D54</f>
         <v>2.9866561298502501</v>
       </c>
       <c r="I45" s="23">
-        <f>'[1]oc-calc'!E54</f>
         <v>14.3835691966099</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" t="str">
-        <f>'[1]oc removal calc 426'!A98</f>
-        <v>I3-A</v>
+      <c r="A46" t="s">
+        <v>158</v>
       </c>
       <c r="B46">
         <v>41</v>
       </c>
       <c r="C46" s="23">
-        <f>'[1]oc removal calc 426'!I98*'[1]oc removal calc 426'!Z98</f>
         <v>29.803281200000001</v>
       </c>
       <c r="D46" s="23"/>
       <c r="F46" s="23">
-        <f>'[1]oc-calc'!B55</f>
         <v>17.704507947759598</v>
       </c>
       <c r="G46" s="23">
-        <f>'[1]oc-calc'!C55</f>
         <v>5.8448626074521899</v>
       </c>
       <c r="H46" s="23">
-        <f>'[1]oc-calc'!D55</f>
         <v>5.5949295377662898</v>
       </c>
       <c r="I46" s="23">
-        <f>'[1]oc-calc'!E55</f>
         <v>30.0573457695148</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" t="str">
-        <f>'[1]oc removal calc 426'!A99</f>
-        <v>I3-B</v>
+      <c r="A47" t="s">
+        <v>159</v>
       </c>
       <c r="B47">
         <v>42</v>
       </c>
       <c r="C47" s="23">
-        <f>'[1]oc removal calc 426'!I99*'[1]oc removal calc 426'!Z99</f>
         <v>27.222272</v>
       </c>
       <c r="D47" s="23"/>
       <c r="F47" s="23">
-        <f>'[1]oc-calc'!B56</f>
         <v>16.637349617478598</v>
       </c>
       <c r="G47" s="23">
-        <f>'[1]oc-calc'!C56</f>
         <v>4.9496144234325996</v>
       </c>
       <c r="H47" s="23">
-        <f>'[1]oc-calc'!D56</f>
         <v>4.9027255049806104</v>
       </c>
       <c r="I47" s="23">
-        <f>'[1]oc-calc'!E56</f>
         <v>27.4027366862097</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" t="str">
-        <f>'[1]oc removal calc 426'!A100</f>
-        <v>B2-A</v>
+      <c r="A48" t="s">
+        <v>160</v>
       </c>
       <c r="B48">
         <v>43</v>
       </c>
       <c r="C48" s="23">
-        <f>'[1]oc removal calc 426'!I100*'[1]oc removal calc 426'!Z100</f>
         <v>22.303134700000001</v>
       </c>
       <c r="D48" s="23"/>
       <c r="F48" s="23">
-        <f>'[1]oc-calc'!B57</f>
         <v>14.558773156429501</v>
       </c>
       <c r="G48" s="23">
-        <f>'[1]oc-calc'!C57</f>
         <v>3.4231449136740699</v>
       </c>
       <c r="H48" s="23">
-        <f>'[1]oc-calc'!D57</f>
         <v>3.6125851863057701</v>
       </c>
       <c r="I48" s="23">
-        <f>'[1]oc-calc'!E57</f>
         <v>22.507826127476299</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" t="str">
-        <f>'[1]oc removal calc 426'!A101</f>
-        <v>B2-B</v>
+      <c r="A49" t="s">
+        <v>161</v>
       </c>
       <c r="B49">
         <v>44</v>
       </c>
       <c r="C49" s="23">
-        <f>'[1]oc removal calc 426'!I101*'[1]oc removal calc 426'!Z101</f>
         <v>11.169627699999999</v>
       </c>
       <c r="D49" s="23"/>
       <c r="F49" s="23">
-        <f>'[1]oc-calc'!B58</f>
         <v>6.4695157867401196</v>
       </c>
       <c r="G49" s="23">
-        <f>'[1]oc-calc'!C58</f>
         <v>1.5172150494338501</v>
       </c>
       <c r="H49" s="23">
-        <f>'[1]oc-calc'!D58</f>
         <v>2.3238986199068399</v>
       </c>
       <c r="I49" s="23">
-        <f>'[1]oc-calc'!E58</f>
         <v>11.2236820111792</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" t="str">
-        <f>'[1]oc removal calc 426'!A102</f>
-        <v>B3-A</v>
+      <c r="A50" t="s">
+        <v>162</v>
       </c>
       <c r="B50">
         <v>45</v>
       </c>
       <c r="C50" s="23">
-        <f>'[1]oc removal calc 426'!I102*'[1]oc removal calc 426'!Z102</f>
         <v>51.508826600000006</v>
       </c>
       <c r="D50" s="23"/>
       <c r="F50" s="23">
-        <f>'[1]oc-calc'!B59</f>
         <v>30.049946834390401</v>
       </c>
       <c r="G50" s="23">
-        <f>'[1]oc-calc'!C59</f>
         <v>11.904879256189</v>
       </c>
       <c r="H50" s="23">
-        <f>'[1]oc-calc'!D59</f>
         <v>9.2526595406910506</v>
       </c>
       <c r="I50" s="23">
-        <f>'[1]oc-calc'!E59</f>
         <v>52.123402176601502</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" t="str">
-        <f>'[1]oc removal calc 426'!A103</f>
-        <v>B3-B</v>
+      <c r="A51" t="s">
+        <v>163</v>
       </c>
       <c r="B51">
         <v>46</v>
       </c>
       <c r="C51" s="23">
-        <f>'[1]oc removal calc 426'!I103*'[1]oc removal calc 426'!Z103</f>
         <v>50.571998399999998</v>
       </c>
       <c r="D51" s="23"/>
       <c r="F51" s="23">
-        <f>'[1]oc-calc'!B60</f>
         <v>30.388644899913398</v>
       </c>
       <c r="G51" s="23">
-        <f>'[1]oc-calc'!C60</f>
         <v>11.607438200328</v>
       </c>
       <c r="H51" s="23">
-        <f>'[1]oc-calc'!D60</f>
         <v>8.3571517250305902</v>
       </c>
       <c r="I51" s="23">
-        <f>'[1]oc-calc'!E60</f>
         <v>51.266235546455299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated readme, edited comments in tc_calc_shiny and oc_calc_shiny
</commit_message>
<xml_diff>
--- a/sunset-calc-performance.xlsx
+++ b/sunset-calc-performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/938fa7904acb035c/Uni Bern/EC-yield_and_charring_calculation_R/R skript development/sunset-calc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinrauber/OneDrive/Uni Bern/EC-yield_and_charring_calculation_R/R skript development/sunset-calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{0D0B52DA-14A4-9140-8D77-65AF9CACC0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E2D439C-F0C8-9640-8E9E-DF7819B4E172}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EDC885-0C85-BE4D-8336-58BB0E78CCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="1" xr2:uid="{37B338B3-0D50-6C40-A204-80C8EAE19EE4}"/>
   </bookViews>
@@ -9226,7 +9226,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -10184,8 +10184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4F56E3-FC80-8F4C-84B3-47DD86B13230}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView zoomScale="139" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -11602,7 +11602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558109FA-2A02-854F-BC43-22E0EACA3551}">
   <dimension ref="A1:AW70"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="161" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="161" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>

</xml_diff>